<commit_message>
Updated Model Through Cash & Equivalents
</commit_message>
<xml_diff>
--- a/Apple 3 Statement Model.xlsx
+++ b/Apple 3 Statement Model.xlsx
@@ -648,7 +648,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="84">
+  <numFmts count="85">
     <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
@@ -733,6 +733,7 @@
     <numFmt numFmtId="240" formatCode="&quot;$&quot;#,##0.0_);\(&quot;$&quot;#,##0.0\)"/>
     <numFmt numFmtId="241" formatCode="0.00\x_);\(0.00\x\);@_)"/>
     <numFmt numFmtId="242" formatCode="0.0"/>
+    <numFmt numFmtId="245" formatCode="0.00%_);\(0.00%\);@_)"/>
   </numFmts>
   <fonts count="105">
     <font>
@@ -2266,7 +2267,7 @@
     <xf numFmtId="0" fontId="97" fillId="0" borderId="0" applyAlignment="0"/>
     <xf numFmtId="231" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2466,6 +2467,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="245" fontId="102" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="212">
     <cellStyle name="$" xfId="1"/>
@@ -3767,10 +3769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L320"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2160" topLeftCell="A302" activePane="bottomLeft"/>
-      <selection activeCell="D220" sqref="D220"/>
-      <selection pane="bottomLeft" activeCell="A320" sqref="A320"/>
+    <sheetView tabSelected="1" topLeftCell="B303" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C321" sqref="C321"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6"/>
@@ -4215,11 +4215,26 @@
       <c r="E22" s="60">
         <v>1616</v>
       </c>
-      <c r="F22"/>
-      <c r="G22"/>
-      <c r="H22"/>
-      <c r="I22"/>
-      <c r="J22"/>
+      <c r="F22" s="96">
+        <f ca="1">F320</f>
+        <v>1539.3080746766282</v>
+      </c>
+      <c r="G22" s="96">
+        <f t="shared" ref="G22:J22" ca="1" si="16">G320</f>
+        <v>1610.1760304807001</v>
+      </c>
+      <c r="H22" s="96">
+        <f t="shared" ca="1" si="16"/>
+        <v>1688.6479972221034</v>
+      </c>
+      <c r="I22" s="96">
+        <f t="shared" ca="1" si="16"/>
+        <v>1779.4169992947996</v>
+      </c>
+      <c r="J22" s="96">
+        <f t="shared" ca="1" si="16"/>
+        <v>1866.6566718140152</v>
+      </c>
     </row>
     <row r="23" spans="2:10">
       <c r="B23" s="3" t="s">
@@ -4239,19 +4254,19 @@
         <v>0</v>
       </c>
       <c r="G23">
-        <f t="shared" ref="G23:J23" ca="1" si="16">G312</f>
+        <f t="shared" ref="G23:J23" ca="1" si="17">G312</f>
         <v>0</v>
       </c>
       <c r="H23">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="17"/>
         <v>0</v>
       </c>
       <c r="I23">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="17"/>
         <v>0</v>
       </c>
       <c r="J23">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -4293,32 +4308,32 @@
         <v>34205</v>
       </c>
       <c r="D25" s="62">
-        <f t="shared" ref="D25:E25" si="17">D21+D24+D23+D22</f>
+        <f t="shared" ref="D25:E25" si="18">D21+D24+D23+D22</f>
         <v>55763</v>
       </c>
       <c r="E25" s="62">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>50155</v>
       </c>
       <c r="F25" s="62">
-        <f t="shared" ref="F25" ca="1" si="18">F21+F24+F23+F22</f>
-        <v>48797.088987599993</v>
+        <f t="shared" ref="F25" ca="1" si="19">F21+F24+F23+F22</f>
+        <v>50336.397062276621</v>
       </c>
       <c r="G25" s="62">
-        <f t="shared" ref="G25" ca="1" si="19">G21+G24+G23+G22</f>
-        <v>51524.534387372238</v>
+        <f t="shared" ref="G25" ca="1" si="20">G21+G24+G23+G22</f>
+        <v>53134.710417852941</v>
       </c>
       <c r="H25" s="62">
-        <f t="shared" ref="H25" ca="1" si="20">H21+H24+H23+H22</f>
-        <v>53847.064773692749</v>
+        <f t="shared" ref="H25" ca="1" si="21">H21+H24+H23+H22</f>
+        <v>55535.712770914855</v>
       </c>
       <c r="I25" s="62">
-        <f t="shared" ref="I25" ca="1" si="21">I21+I24+I23+I22</f>
-        <v>56511.430285172188</v>
+        <f t="shared" ref="I25" ca="1" si="22">I21+I24+I23+I22</f>
+        <v>58290.847284466989</v>
       </c>
       <c r="J25" s="62">
-        <f t="shared" ref="J25" ca="1" si="22">J21+J24+J23+J22</f>
-        <v>59573.419689579961</v>
+        <f t="shared" ref="J25" ca="1" si="23">J21+J24+J23+J22</f>
+        <v>61440.076361393978</v>
       </c>
     </row>
     <row r="26" spans="2:10">
@@ -4336,23 +4351,23 @@
       </c>
       <c r="F26" s="72">
         <f ca="1">-(F25*F41)</f>
-        <v>-12833.634403738799</v>
+        <v>-13238.472427378752</v>
       </c>
       <c r="G26" s="72">
         <f ca="1">-(G25*G41)</f>
-        <v>-13396.378940716782</v>
+        <v>-13815.024708641766</v>
       </c>
       <c r="H26" s="72">
         <f ca="1">-(H25*H41)</f>
-        <v>-14000.236841160115</v>
+        <v>-14439.285320437863</v>
       </c>
       <c r="I26" s="72">
         <f ca="1">-(I25*I41)</f>
-        <v>-14692.971874144769</v>
+        <v>-15155.620293961418</v>
       </c>
       <c r="J26" s="70">
         <f ca="1">-(J25*J41)</f>
-        <v>-15489.089119290791</v>
+        <v>-15974.419853962434</v>
       </c>
     </row>
     <row r="27" spans="2:10">
@@ -4364,32 +4379,32 @@
         <v>25922</v>
       </c>
       <c r="D27" s="62">
-        <f t="shared" ref="D27:E27" si="23">D25+D26</f>
+        <f t="shared" ref="D27:E27" si="24">D25+D26</f>
         <v>41733</v>
       </c>
       <c r="E27" s="62">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>37037</v>
       </c>
       <c r="F27" s="62">
-        <f t="shared" ref="F27" ca="1" si="24">F25+F26</f>
-        <v>35963.454583861196</v>
+        <f t="shared" ref="F27" ca="1" si="25">F25+F26</f>
+        <v>37097.92463489787</v>
       </c>
       <c r="G27" s="62">
-        <f t="shared" ref="G27" ca="1" si="25">G25+G26</f>
-        <v>38128.155446655452</v>
+        <f t="shared" ref="G27" ca="1" si="26">G25+G26</f>
+        <v>39319.685709211175</v>
       </c>
       <c r="H27" s="62">
-        <f t="shared" ref="H27" ca="1" si="26">H25+H26</f>
-        <v>39846.827932532637</v>
+        <f t="shared" ref="H27" ca="1" si="27">H25+H26</f>
+        <v>41096.427450476993</v>
       </c>
       <c r="I27" s="62">
-        <f t="shared" ref="I27" ca="1" si="27">I25+I26</f>
-        <v>41818.458411027415</v>
+        <f t="shared" ref="I27" ca="1" si="28">I25+I26</f>
+        <v>43135.226990505573</v>
       </c>
       <c r="J27" s="62">
-        <f t="shared" ref="J27" ca="1" si="28">J25+J26</f>
-        <v>44084.330570289167</v>
+        <f t="shared" ref="J27" ca="1" si="29">J25+J26</f>
+        <v>45465.656507431544</v>
       </c>
     </row>
     <row r="28" spans="2:10">
@@ -4430,11 +4445,11 @@
         <v>6331</v>
       </c>
       <c r="D30" s="64">
-        <f t="shared" ref="D30:E30" si="29">D31-D29</f>
+        <f t="shared" ref="D30:E30" si="30">D31-D29</f>
         <v>10537</v>
       </c>
       <c r="E30" s="64">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>6331</v>
       </c>
       <c r="F30"/>
@@ -4537,23 +4552,23 @@
         <v>9.2020855163953197E-2</v>
       </c>
       <c r="F37" s="65">
-        <f t="shared" ref="F37:J37" si="30">F16/E16-1</f>
+        <f t="shared" ref="F37:J37" si="31">F16/E16-1</f>
         <v>4.893831490258016E-2</v>
       </c>
       <c r="G37" s="65">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>5.1686665077156135E-2</v>
       </c>
       <c r="H37" s="65">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>4.4794523389385388E-2</v>
       </c>
       <c r="I37" s="65">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>4.9184292806689678E-2</v>
       </c>
       <c r="J37" s="65">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>5.3874658624808891E-2</v>
       </c>
     </row>
@@ -4566,11 +4581,11 @@
         <v>0.40478895878945764</v>
       </c>
       <c r="D38" s="65">
-        <f t="shared" ref="D38:E38" si="31">D18/D16</f>
+        <f t="shared" ref="D38:E38" si="32">D18/D16</f>
         <v>0.43871239808827661</v>
       </c>
       <c r="E38" s="65">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.37624480720847231</v>
       </c>
       <c r="F38" s="56">
@@ -4726,19 +4741,19 @@
         <v>7145.3176115999995</v>
       </c>
       <c r="G44" s="96">
-        <f t="shared" ref="G44:J44" si="32">-(G177+G164)</f>
+        <f t="shared" ref="G44:J44" si="33">-(G177+G164)</f>
         <v>7540.5401478143021</v>
       </c>
       <c r="H44" s="96">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>7682.1924442956242</v>
       </c>
       <c r="I44" s="96">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>7792.0651309652267</v>
       </c>
       <c r="J44" s="96">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>8007.2119367516216</v>
       </c>
     </row>
@@ -4760,19 +4775,19 @@
         <v>2212.6002930107998</v>
       </c>
       <c r="G45" s="96">
-        <f t="shared" ref="G45:J45" si="33">G231</f>
+        <f t="shared" ref="G45:J45" si="34">G231</f>
         <v>2187.0654505218836</v>
       </c>
       <c r="H45" s="96">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>2285.0340049994029</v>
       </c>
       <c r="I45" s="96">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>2397.4217865745363</v>
       </c>
       <c r="J45" s="96">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>2526.5820669059194</v>
       </c>
     </row>
@@ -4785,31 +4800,31 @@
         <v>36772</v>
       </c>
       <c r="D46" s="62">
-        <f t="shared" ref="D46:J46" si="34">D21+D45+D44</f>
+        <f t="shared" ref="D46:J46" si="35">D21+D45+D44</f>
         <v>60258</v>
       </c>
       <c r="E46" s="62">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>58009</v>
       </c>
       <c r="F46" s="62">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>58479.006892210789</v>
       </c>
       <c r="G46" s="62">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>61576.139985708425</v>
       </c>
       <c r="H46" s="62">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>64138.291222987777</v>
       </c>
       <c r="I46" s="62">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>67024.917202711949</v>
       </c>
       <c r="J46" s="62">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>70431.2136932375</v>
       </c>
     </row>
@@ -4841,7 +4856,7 @@
     </row>
     <row r="49" spans="2:10">
       <c r="B49" s="3" t="str">
-        <f t="shared" ref="B49:B50" si="35">B13</f>
+        <f t="shared" ref="B49:B50" si="36">B13</f>
         <v xml:space="preserve">Fiscal year  </v>
       </c>
       <c r="C49" s="58">
@@ -4861,25 +4876,25 @@
         <v>2014</v>
       </c>
       <c r="G49" s="59">
-        <f t="shared" ref="G49:J49" si="36">F49+1</f>
+        <f t="shared" ref="G49:J49" si="37">F49+1</f>
         <v>2015</v>
       </c>
       <c r="H49" s="59">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>2016</v>
       </c>
       <c r="I49" s="59">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>2017</v>
       </c>
       <c r="J49" s="59">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>2018</v>
       </c>
     </row>
     <row r="50" spans="2:10">
       <c r="B50" s="15" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>Fiscal year end date</v>
       </c>
       <c r="C50" s="34">
@@ -4899,19 +4914,19 @@
         <v>41912</v>
       </c>
       <c r="G50" s="57">
-        <f t="shared" ref="G50:J50" si="37">EOMONTH(F50,12)</f>
+        <f t="shared" ref="G50:J50" si="38">EOMONTH(F50,12)</f>
         <v>42277</v>
       </c>
       <c r="H50" s="57">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>42643</v>
       </c>
       <c r="I50" s="57">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>43008</v>
       </c>
       <c r="J50" s="57">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>43373</v>
       </c>
     </row>
@@ -4946,19 +4961,19 @@
         <v>97967.925119999971</v>
       </c>
       <c r="G52" s="70">
-        <f t="shared" ref="G52:J52" si="38">(G62*G72)/1000</f>
+        <f t="shared" ref="G52:J52" si="39">(G62*G72)/1000</f>
         <v>105021.61572863998</v>
       </c>
       <c r="H52" s="70">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>108172.26420049919</v>
       </c>
       <c r="I52" s="70">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>111417.43212651416</v>
       </c>
       <c r="J52" s="70">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>114759.95509030961</v>
       </c>
     </row>
@@ -4980,19 +4995,19 @@
         <v>31590.195779999995</v>
       </c>
       <c r="G53" s="70">
-        <f t="shared" ref="G53:J53" si="39">(G64*G74)/1000</f>
+        <f t="shared" ref="G53:J53" si="40">(G64*G74)/1000</f>
         <v>31590.195779999995</v>
       </c>
       <c r="H53" s="70">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>31590.195779999995</v>
       </c>
       <c r="I53" s="70">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>31590.195779999995</v>
       </c>
       <c r="J53" s="70">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>31590.195779999995</v>
       </c>
     </row>
@@ -5014,19 +5029,19 @@
         <v>20902.958999999999</v>
       </c>
       <c r="G54" s="70">
-        <f t="shared" ref="G54:J54" si="40">(G66*G76)/1000</f>
+        <f t="shared" ref="G54:J54" si="41">(G66*G76)/1000</f>
         <v>18860.217331724998</v>
       </c>
       <c r="H54" s="70">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>18860.217331724998</v>
       </c>
       <c r="I54" s="70">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>18860.217331724998</v>
       </c>
       <c r="J54" s="70">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>18860.217331724998</v>
       </c>
     </row>
@@ -5048,19 +5063,19 @@
         <v>3275.1675</v>
       </c>
       <c r="G55" s="70">
-        <f t="shared" ref="G55:J55" si="41">(G68*G78)/1000</f>
+        <f t="shared" ref="G55:J55" si="42">(G68*G78)/1000</f>
         <v>2736.566204625</v>
       </c>
       <c r="H55" s="70">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>2326.0812739312501</v>
       </c>
       <c r="I55" s="70">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>1977.1690828415624</v>
       </c>
       <c r="J55" s="70">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>1680.5937204153279</v>
       </c>
     </row>
@@ -5082,19 +5097,19 @@
         <v>19261.2</v>
       </c>
       <c r="G56" s="70">
-        <f t="shared" ref="G56:J56" si="42">F56*(1+G81)</f>
+        <f t="shared" ref="G56:J56" si="43">F56*(1+G81)</f>
         <v>23113.439999999999</v>
       </c>
       <c r="H56" s="70">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>27736.127999999997</v>
       </c>
       <c r="I56" s="70">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>33283.353599999995</v>
       </c>
       <c r="J56" s="70">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>39940.02431999999</v>
       </c>
     </row>
@@ -5116,19 +5131,19 @@
         <v>6276.6</v>
       </c>
       <c r="G57" s="70">
-        <f t="shared" ref="G57:J57" si="43">F57*(1+G82)</f>
+        <f t="shared" ref="G57:J57" si="44">F57*(1+G82)</f>
         <v>7218.09</v>
       </c>
       <c r="H57" s="70">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>8300.8035</v>
       </c>
       <c r="I57" s="70">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>9545.9240249999984</v>
       </c>
       <c r="J57" s="70">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>10977.812628749998</v>
       </c>
     </row>
@@ -5141,31 +5156,31 @@
         <v>108249</v>
       </c>
       <c r="D58" s="64">
-        <f t="shared" ref="D58:E58" si="44">SUM(D52:D57)</f>
+        <f t="shared" ref="D58:E58" si="45">SUM(D52:D57)</f>
         <v>156508</v>
       </c>
       <c r="E58" s="64">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>170910</v>
       </c>
       <c r="F58" s="64">
-        <f t="shared" ref="F58" si="45">SUM(F52:F57)</f>
+        <f t="shared" ref="F58" si="46">SUM(F52:F57)</f>
         <v>179274.04739999998</v>
       </c>
       <c r="G58" s="64">
-        <f t="shared" ref="G58" si="46">SUM(G52:G57)</f>
+        <f t="shared" ref="G58" si="47">SUM(G52:G57)</f>
         <v>188540.12504498998</v>
       </c>
       <c r="H58" s="64">
-        <f t="shared" ref="H58" si="47">SUM(H52:H57)</f>
+        <f t="shared" ref="H58" si="48">SUM(H52:H57)</f>
         <v>196985.69008615543</v>
       </c>
       <c r="I58" s="64">
-        <f t="shared" ref="I58" si="48">SUM(I52:I57)</f>
+        <f t="shared" ref="I58" si="49">SUM(I52:I57)</f>
         <v>206674.29194608072</v>
       </c>
       <c r="J58" s="64">
-        <f t="shared" ref="J58" si="49">SUM(J52:J57)</f>
+        <f t="shared" ref="J58" si="50">SUM(J52:J57)</f>
         <v>217808.79887119992</v>
       </c>
     </row>
@@ -5183,23 +5198,23 @@
         <v>9.2020855163953197E-2</v>
       </c>
       <c r="F59" s="65">
-        <f t="shared" ref="F59:J59" si="50">F58/E58-1</f>
+        <f t="shared" ref="F59:J59" si="51">F58/E58-1</f>
         <v>4.893831490258016E-2</v>
       </c>
       <c r="G59" s="65">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>5.1686665077156135E-2</v>
       </c>
       <c r="H59" s="65">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>4.4794523389385388E-2</v>
       </c>
       <c r="I59" s="65">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>4.9184292806689678E-2</v>
       </c>
       <c r="J59" s="65">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>5.3874658624808891E-2</v>
       </c>
     </row>
@@ -5245,19 +5260,19 @@
         <v>167987.32599999997</v>
       </c>
       <c r="G62" s="72">
-        <f t="shared" ref="G62:J62" si="51">F62*(1+G63)</f>
+        <f t="shared" ref="G62:J62" si="52">F62*(1+G63)</f>
         <v>180082.41347199999</v>
       </c>
       <c r="H62" s="72">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>185484.88587616</v>
       </c>
       <c r="I62" s="72">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>191049.4324524448</v>
       </c>
       <c r="J62" s="72">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>196780.91542601815</v>
       </c>
     </row>
@@ -5308,19 +5323,19 @@
         <v>71672.296999999991</v>
       </c>
       <c r="G64" s="72">
-        <f t="shared" ref="G64:J64" si="52">F64*(G65+1)</f>
+        <f t="shared" ref="G64:J64" si="53">F64*(G65+1)</f>
         <v>71672.296999999991</v>
       </c>
       <c r="H64" s="72">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>71672.296999999991</v>
       </c>
       <c r="I64" s="72">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>71672.296999999991</v>
       </c>
       <c r="J64" s="72">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>71672.296999999991</v>
       </c>
     </row>
@@ -5371,19 +5386,19 @@
         <v>15899.793000000003</v>
       </c>
       <c r="G66" s="72">
-        <f t="shared" ref="G66:J66" si="53">F66*(1+G67)</f>
+        <f t="shared" ref="G66:J66" si="54">F66*(1+G67)</f>
         <v>15343.300245000002</v>
       </c>
       <c r="H66" s="72">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>15343.300245000002</v>
       </c>
       <c r="I66" s="72">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>15343.300245000002</v>
       </c>
       <c r="J66" s="72">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>15343.300245000002</v>
       </c>
     </row>
@@ -5434,19 +5449,19 @@
         <v>19784.25</v>
       </c>
       <c r="G68" s="72">
-        <f t="shared" ref="G68:J68" si="54">F68*(1+G69)</f>
+        <f t="shared" ref="G68:J68" si="55">F68*(1+G69)</f>
         <v>16816.612499999999</v>
       </c>
       <c r="H68" s="72">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>14294.120625</v>
       </c>
       <c r="I68" s="72">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>12150.00253125</v>
       </c>
       <c r="J68" s="72">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>10327.502151562499</v>
       </c>
     </row>
@@ -5512,11 +5527,11 @@
         <v>636.27183821393487</v>
       </c>
       <c r="D72" s="66">
-        <f t="shared" ref="D72:E72" si="55">D52/D62*1000</f>
+        <f t="shared" ref="D72:E72" si="56">D52/D62*1000</f>
         <v>629.30441597492131</v>
       </c>
       <c r="E72" s="66">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>607.48584092588032</v>
       </c>
       <c r="F72" s="66">
@@ -5524,19 +5539,19 @@
         <v>583.18640728884509</v>
       </c>
       <c r="G72" s="66">
-        <f t="shared" ref="G72:J72" si="56">F72*(1+G73)</f>
+        <f t="shared" ref="G72:J72" si="57">F72*(1+G73)</f>
         <v>583.18640728884509</v>
       </c>
       <c r="H72" s="66">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>583.18640728884509</v>
       </c>
       <c r="I72" s="66">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>583.18640728884509</v>
       </c>
       <c r="J72" s="66">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>583.18640728884509</v>
       </c>
     </row>
@@ -5578,11 +5593,11 @@
         <v>591.71451503364824</v>
       </c>
       <c r="D74" s="66">
-        <f t="shared" ref="D74:E74" si="57">D53/D64*1000</f>
+        <f t="shared" ref="D74:E74" si="58">D53/D64*1000</f>
         <v>530.69799348310755</v>
       </c>
       <c r="E74" s="66">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>450.21328115101431</v>
       </c>
       <c r="F74" s="66">
@@ -5590,19 +5605,19 @@
         <v>440.758802246843</v>
       </c>
       <c r="G74" s="66">
-        <f t="shared" ref="G74:J74" si="58">F74*(1+G75)</f>
+        <f t="shared" ref="G74:J74" si="59">F74*(1+G75)</f>
         <v>440.758802246843</v>
       </c>
       <c r="H74" s="66">
-        <f t="shared" si="58"/>
+        <f t="shared" si="59"/>
         <v>440.758802246843</v>
       </c>
       <c r="I74" s="66">
-        <f t="shared" si="58"/>
+        <f t="shared" si="59"/>
         <v>440.758802246843</v>
       </c>
       <c r="J74" s="66">
-        <f t="shared" si="58"/>
+        <f t="shared" si="59"/>
         <v>440.758802246843</v>
       </c>
     </row>
@@ -5644,11 +5659,11 @@
         <v>1301.6432626232445</v>
       </c>
       <c r="D76" s="66">
-        <f t="shared" ref="D76:E76" si="59">D54/D66*1000</f>
+        <f t="shared" ref="D76:E76" si="60">D54/D66*1000</f>
         <v>1278.8302676506225</v>
       </c>
       <c r="E76" s="66">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>1314.6686249311545</v>
       </c>
       <c r="F76" s="66">
@@ -5656,19 +5671,19 @@
         <v>1314.6686249311545</v>
       </c>
       <c r="G76" s="66">
-        <f t="shared" ref="G76:J76" si="60">F76*(1+G77)</f>
+        <f t="shared" ref="G76:J76" si="61">F76*(1+G77)</f>
         <v>1229.2151643106295</v>
       </c>
       <c r="H76" s="66">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>1229.2151643106295</v>
       </c>
       <c r="I76" s="66">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>1229.2151643106295</v>
       </c>
       <c r="J76" s="66">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>1229.2151643106295</v>
       </c>
     </row>
@@ -5710,11 +5725,11 @@
         <v>174.87095260441106</v>
       </c>
       <c r="D78" s="66">
-        <f t="shared" ref="D78:E78" si="61">D55/D68*1000</f>
+        <f t="shared" ref="D78:E78" si="62">D55/D68*1000</f>
         <v>159.67581401962178</v>
       </c>
       <c r="E78" s="66">
-        <f t="shared" si="61"/>
+        <f t="shared" si="62"/>
         <v>167.21634633610068</v>
       </c>
       <c r="F78" s="66">
@@ -5722,19 +5737,19 @@
         <v>165.54418287273967</v>
       </c>
       <c r="G78" s="66">
-        <f t="shared" ref="G78:J78" si="62">F78*(1+G79)</f>
+        <f t="shared" ref="G78:J78" si="63">F78*(1+G79)</f>
         <v>162.7299317639031</v>
       </c>
       <c r="H78" s="66">
-        <f t="shared" si="62"/>
+        <f t="shared" si="63"/>
         <v>162.7299317639031</v>
       </c>
       <c r="I78" s="66">
-        <f t="shared" si="62"/>
+        <f t="shared" si="63"/>
         <v>162.7299317639031</v>
       </c>
       <c r="J78" s="66">
-        <f t="shared" si="62"/>
+        <f t="shared" si="63"/>
         <v>162.7299317639031</v>
       </c>
     </row>
@@ -5868,31 +5883,31 @@
       </c>
       <c r="C85" s="80"/>
       <c r="D85" s="80">
-        <f t="shared" ref="D85:J86" si="63">D13</f>
+        <f t="shared" ref="D85:J86" si="64">D13</f>
         <v>2012</v>
       </c>
       <c r="E85" s="80">
-        <f t="shared" si="63"/>
+        <f t="shared" si="64"/>
         <v>2013</v>
       </c>
       <c r="F85" s="81">
-        <f t="shared" si="63"/>
+        <f t="shared" si="64"/>
         <v>2014</v>
       </c>
       <c r="G85" s="81">
-        <f t="shared" si="63"/>
+        <f t="shared" si="64"/>
         <v>2015</v>
       </c>
       <c r="H85" s="81">
-        <f t="shared" si="63"/>
+        <f t="shared" si="64"/>
         <v>2016</v>
       </c>
       <c r="I85" s="81">
-        <f t="shared" si="63"/>
+        <f t="shared" si="64"/>
         <v>2017</v>
       </c>
       <c r="J85" s="81">
-        <f t="shared" si="63"/>
+        <f t="shared" si="64"/>
         <v>2018</v>
       </c>
     </row>
@@ -5903,31 +5918,31 @@
       </c>
       <c r="C86" s="82"/>
       <c r="D86" s="82">
-        <f t="shared" si="63"/>
+        <f t="shared" si="64"/>
         <v>41181</v>
       </c>
       <c r="E86" s="82">
-        <f t="shared" si="63"/>
+        <f t="shared" si="64"/>
         <v>41545</v>
       </c>
       <c r="F86" s="82">
-        <f t="shared" si="63"/>
+        <f t="shared" si="64"/>
         <v>41912</v>
       </c>
       <c r="G86" s="82">
-        <f t="shared" si="63"/>
+        <f t="shared" si="64"/>
         <v>42277</v>
       </c>
       <c r="H86" s="82">
-        <f t="shared" si="63"/>
+        <f t="shared" si="64"/>
         <v>42643</v>
       </c>
       <c r="I86" s="82">
-        <f t="shared" si="63"/>
+        <f t="shared" si="64"/>
         <v>43008</v>
       </c>
       <c r="J86" s="82">
-        <f t="shared" si="63"/>
+        <f t="shared" si="64"/>
         <v>43373</v>
       </c>
     </row>
@@ -5944,11 +5959,26 @@
         <f>14259+26287+106215</f>
         <v>146761</v>
       </c>
-      <c r="F87"/>
-      <c r="G87"/>
-      <c r="H87"/>
-      <c r="I87"/>
-      <c r="J87"/>
+      <c r="F87" s="96">
+        <f ca="1">E87+F290</f>
+        <v>152133.77178186952</v>
+      </c>
+      <c r="G87" s="96">
+        <f t="shared" ref="G87:J87" ca="1" si="65">F87+G290</f>
+        <v>160521.76811729561</v>
+      </c>
+      <c r="H87" s="96">
+        <f t="shared" ca="1" si="65"/>
+        <v>167371.04687728541</v>
+      </c>
+      <c r="I87" s="96">
+        <f t="shared" ca="1" si="65"/>
+        <v>178146.81706348865</v>
+      </c>
+      <c r="J87" s="96">
+        <f t="shared" ca="1" si="65"/>
+        <v>184310.78911391232</v>
+      </c>
     </row>
     <row r="88" spans="1:10">
       <c r="B88" s="3" t="s">
@@ -5966,19 +5996,19 @@
         <v>13535.190578699998</v>
       </c>
       <c r="G88" s="109">
-        <f t="shared" ref="G88:J88" si="64">G126</f>
+        <f t="shared" ref="G88:J88" si="66">G126</f>
         <v>14329.049503419239</v>
       </c>
       <c r="H88" s="109">
-        <f t="shared" si="64"/>
+        <f t="shared" si="66"/>
         <v>14970.912446547813</v>
       </c>
       <c r="I88" s="109">
-        <f t="shared" si="64"/>
+        <f t="shared" si="66"/>
         <v>15707.246187902134</v>
       </c>
       <c r="J88" s="109">
-        <f t="shared" si="64"/>
+        <f t="shared" si="66"/>
         <v>16553.468714211194</v>
       </c>
     </row>
@@ -5998,19 +6028,19 @@
         <v>1804.2140130335999</v>
       </c>
       <c r="G89" s="96">
-        <f t="shared" ref="G89:J89" si="65">G134</f>
+        <f t="shared" ref="G89:J89" si="67">G134</f>
         <v>1947.4309515897016</v>
       </c>
       <c r="H89" s="96">
-        <f t="shared" si="65"/>
+        <f t="shared" si="67"/>
         <v>2034.6651928998995</v>
       </c>
       <c r="I89" s="96">
-        <f t="shared" si="65"/>
+        <f t="shared" si="67"/>
         <v>2134.7387615110679</v>
       </c>
       <c r="J89" s="96">
-        <f t="shared" si="65"/>
+        <f t="shared" si="67"/>
         <v>2249.7470835406243</v>
       </c>
     </row>
@@ -6030,19 +6060,19 @@
         <v>3453</v>
       </c>
       <c r="G90" s="96">
-        <f t="shared" ref="G90:J90" si="66">G192</f>
+        <f t="shared" ref="G90:J90" si="68">G192</f>
         <v>3453</v>
       </c>
       <c r="H90" s="96">
-        <f t="shared" si="66"/>
+        <f t="shared" si="68"/>
         <v>3453</v>
       </c>
       <c r="I90" s="96">
-        <f t="shared" si="66"/>
+        <f t="shared" si="68"/>
         <v>3453</v>
       </c>
       <c r="J90" s="96">
-        <f t="shared" si="66"/>
+        <f t="shared" si="68"/>
         <v>3453</v>
       </c>
     </row>
@@ -6064,19 +6094,19 @@
         <v>14421</v>
       </c>
       <c r="G91" s="96">
-        <f t="shared" ref="G91:J91" si="67">G187</f>
+        <f t="shared" ref="G91:J91" si="69">G187</f>
         <v>14421</v>
       </c>
       <c r="H91" s="96">
-        <f t="shared" si="67"/>
+        <f t="shared" si="69"/>
         <v>14421</v>
       </c>
       <c r="I91" s="96">
-        <f t="shared" si="67"/>
+        <f t="shared" si="69"/>
         <v>14421</v>
       </c>
       <c r="J91" s="96">
-        <f t="shared" si="67"/>
+        <f t="shared" si="69"/>
         <v>14421</v>
       </c>
     </row>
@@ -6096,19 +6126,19 @@
         <v>19465.3847584</v>
       </c>
       <c r="G92" s="96">
-        <f t="shared" ref="G92:J92" si="68">G173</f>
+        <f t="shared" ref="G92:J92" si="70">G173</f>
         <v>23656.631738150129</v>
       </c>
       <c r="H92" s="96">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>28035.623628765366</v>
       </c>
       <c r="I92" s="96">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>32629.993138726739</v>
       </c>
       <c r="J92" s="96">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>37471.882737633518</v>
       </c>
     </row>
@@ -6130,19 +6160,19 @@
         <v>4706</v>
       </c>
       <c r="G93" s="96">
-        <f t="shared" ref="G93:J93" si="69">G161</f>
+        <f t="shared" ref="G93:J93" si="71">G161</f>
         <v>3721</v>
       </c>
       <c r="H93" s="96">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>2888</v>
       </c>
       <c r="I93" s="96">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>2282</v>
       </c>
       <c r="J93" s="96">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>1848</v>
       </c>
     </row>
@@ -6162,19 +6192,19 @@
         <v>5146</v>
       </c>
       <c r="G94" s="96">
-        <f t="shared" ref="G94:J94" si="70">G197</f>
+        <f t="shared" ref="G94:J94" si="72">G197</f>
         <v>5146</v>
       </c>
       <c r="H94" s="96">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>5146</v>
       </c>
       <c r="I94" s="96">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>5146</v>
       </c>
       <c r="J94" s="96">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>5146</v>
       </c>
     </row>
@@ -6192,24 +6222,24 @@
         <v>207000</v>
       </c>
       <c r="F95" s="89">
-        <f t="shared" ref="F95:J95" si="71">SUM(F87:F94)</f>
-        <v>62530.789350133593</v>
+        <f t="shared" ref="F95:J95" ca="1" si="73">SUM(F87:F94)</f>
+        <v>214664.56113200312</v>
       </c>
       <c r="G95" s="89">
-        <f t="shared" si="71"/>
-        <v>66674.112193159061</v>
+        <f t="shared" ca="1" si="73"/>
+        <v>227195.88031045464</v>
       </c>
       <c r="H95" s="89">
-        <f t="shared" si="71"/>
-        <v>70949.201268213073</v>
+        <f t="shared" ca="1" si="73"/>
+        <v>238320.24814549851</v>
       </c>
       <c r="I95" s="89">
-        <f t="shared" si="71"/>
-        <v>75773.978088139949</v>
+        <f t="shared" ca="1" si="73"/>
+        <v>253920.79515162861</v>
       </c>
       <c r="J95" s="89">
-        <f t="shared" si="71"/>
-        <v>81143.098535385332</v>
+        <f t="shared" ca="1" si="73"/>
+        <v>265453.88764929766</v>
       </c>
     </row>
     <row r="96" spans="1:10">
@@ -6239,19 +6269,19 @@
         <v>22890.965290363798</v>
       </c>
       <c r="G97" s="96">
-        <f t="shared" ref="G97:J97" si="72">G142</f>
+        <f t="shared" ref="G97:J97" si="74">G142</f>
         <v>24313.380365301728</v>
       </c>
       <c r="H97" s="96">
-        <f t="shared" si="72"/>
+        <f t="shared" si="74"/>
         <v>25402.486650750256</v>
       </c>
       <c r="I97" s="96">
-        <f t="shared" si="72"/>
+        <f t="shared" si="74"/>
         <v>26651.889992198783</v>
       </c>
       <c r="J97" s="96">
-        <f t="shared" si="72"/>
+        <f t="shared" si="74"/>
         <v>28087.751467234459</v>
       </c>
     </row>
@@ -6273,19 +6303,19 @@
         <v>23843.448304199999</v>
       </c>
       <c r="G98" s="96">
-        <f t="shared" ref="G98:J98" si="73">G150</f>
+        <f t="shared" ref="G98:J98" si="75">G150</f>
         <v>23850.325818191232</v>
       </c>
       <c r="H98" s="96">
-        <f t="shared" si="73"/>
+        <f t="shared" si="75"/>
         <v>23835.268500424805</v>
       </c>
       <c r="I98" s="96">
-        <f t="shared" si="73"/>
+        <f t="shared" si="75"/>
         <v>23974.217865745366</v>
       </c>
       <c r="J98" s="96">
-        <f t="shared" si="73"/>
+        <f t="shared" si="75"/>
         <v>23958.96787583199</v>
       </c>
     </row>
@@ -6337,19 +6367,19 @@
         <v>16960</v>
       </c>
       <c r="G100" s="96">
-        <f t="shared" ref="G100:J100" si="74">G212</f>
+        <f t="shared" ref="G100:J100" si="76">G212</f>
         <v>16960</v>
       </c>
       <c r="H100" s="96">
-        <f t="shared" si="74"/>
+        <f t="shared" si="76"/>
         <v>14460</v>
       </c>
       <c r="I100" s="96">
-        <f t="shared" si="74"/>
+        <f t="shared" si="76"/>
         <v>14460</v>
       </c>
       <c r="J100" s="96">
-        <f t="shared" si="74"/>
+        <f t="shared" si="76"/>
         <v>8460</v>
       </c>
     </row>
@@ -6369,19 +6399,19 @@
         <v>23208</v>
       </c>
       <c r="G101" s="96">
-        <f t="shared" ref="G101:J101" si="75">G202</f>
+        <f t="shared" ref="G101:J101" si="77">G202</f>
         <v>26208</v>
       </c>
       <c r="H101" s="96">
-        <f t="shared" si="75"/>
+        <f t="shared" si="77"/>
         <v>29208</v>
       </c>
       <c r="I101" s="96">
-        <f t="shared" si="75"/>
+        <f t="shared" si="77"/>
         <v>32208</v>
       </c>
       <c r="J101" s="96">
-        <f t="shared" si="75"/>
+        <f t="shared" si="77"/>
         <v>35208</v>
       </c>
     </row>
@@ -6399,23 +6429,23 @@
         <v>83451</v>
       </c>
       <c r="F102" s="89">
-        <f t="shared" ref="F102:J102" ca="1" si="76">SUM(F97:F101)</f>
+        <f t="shared" ref="F102:J102" ca="1" si="78">SUM(F97:F101)</f>
         <v>86902.413594563797</v>
       </c>
       <c r="G102" s="89">
-        <f t="shared" ca="1" si="76"/>
+        <f t="shared" ca="1" si="78"/>
         <v>91331.706183492963</v>
       </c>
       <c r="H102" s="89">
-        <f t="shared" ca="1" si="76"/>
+        <f t="shared" ca="1" si="78"/>
         <v>92905.755151175064</v>
       </c>
       <c r="I102" s="89">
-        <f t="shared" ca="1" si="76"/>
+        <f t="shared" ca="1" si="78"/>
         <v>97294.107857944153</v>
       </c>
       <c r="J102" s="89">
-        <f t="shared" ca="1" si="76"/>
+        <f t="shared" ca="1" si="78"/>
         <v>95714.719343066448</v>
       </c>
     </row>
@@ -6446,19 +6476,19 @@
         <v>21976.600293010801</v>
       </c>
       <c r="G104" s="96">
-        <f t="shared" ref="G104:J104" si="77">G228</f>
+        <f t="shared" ref="G104:J104" si="79">G228</f>
         <v>24163.665743532685</v>
       </c>
       <c r="H104" s="96">
-        <f t="shared" si="77"/>
+        <f t="shared" si="79"/>
         <v>26448.69974853209</v>
       </c>
       <c r="I104" s="96">
-        <f t="shared" si="77"/>
+        <f t="shared" si="79"/>
         <v>28846.121535106628</v>
       </c>
       <c r="J104" s="96">
-        <f t="shared" si="77"/>
+        <f t="shared" si="79"/>
         <v>31372.703602012545</v>
       </c>
     </row>
@@ -6478,19 +6508,19 @@
         <v>-23968</v>
       </c>
       <c r="G105" s="96">
-        <f t="shared" ref="G105:J105" si="78">G237</f>
+        <f t="shared" ref="G105:J105" si="80">G237</f>
         <v>-47936</v>
       </c>
       <c r="H105" s="96">
-        <f t="shared" si="78"/>
+        <f t="shared" si="80"/>
         <v>-71904</v>
       </c>
       <c r="I105" s="96">
-        <f t="shared" si="78"/>
+        <f t="shared" si="80"/>
         <v>-95872</v>
       </c>
       <c r="J105" s="96">
-        <f t="shared" si="78"/>
+        <f t="shared" si="80"/>
         <v>-119840</v>
       </c>
     </row>
@@ -6507,23 +6537,23 @@
       </c>
       <c r="F106" s="52">
         <f ca="1">F249</f>
-        <v>129430.41820870283</v>
+        <v>130224.54724442851</v>
       </c>
       <c r="G106" s="52">
-        <f t="shared" ref="G106:J106" ca="1" si="79">G249</f>
-        <v>158407.81634816097</v>
+        <f t="shared" ref="G106:J106" ca="1" si="81">G249</f>
+        <v>160107.508383429</v>
       </c>
       <c r="H106" s="52">
-        <f t="shared" ca="1" si="79"/>
-        <v>188691.40557688577</v>
+        <f t="shared" ca="1" si="81"/>
+        <v>191340.79324579198</v>
       </c>
       <c r="I106" s="52">
-        <f t="shared" ca="1" si="79"/>
-        <v>220473.4339692666</v>
+        <f t="shared" ca="1" si="81"/>
+        <v>224123.56575856666</v>
       </c>
       <c r="J106" s="52">
-        <f t="shared" ca="1" si="79"/>
-        <v>253977.52520268637</v>
+        <f t="shared" ca="1" si="81"/>
+        <v>258677.46470433022</v>
       </c>
     </row>
     <row r="107" spans="2:10">
@@ -6542,19 +6572,19 @@
         <v>-471</v>
       </c>
       <c r="G107" s="96">
-        <f t="shared" ref="G107:J107" si="80">G258</f>
+        <f t="shared" ref="G107:J107" si="82">G258</f>
         <v>-471</v>
       </c>
       <c r="H107" s="96">
-        <f t="shared" si="80"/>
+        <f t="shared" si="82"/>
         <v>-471</v>
       </c>
       <c r="I107" s="96">
-        <f t="shared" si="80"/>
+        <f t="shared" si="82"/>
         <v>-471</v>
       </c>
       <c r="J107" s="96">
-        <f t="shared" si="80"/>
+        <f t="shared" si="82"/>
         <v>-471</v>
       </c>
     </row>
@@ -6572,24 +6602,24 @@
         <v>123549</v>
       </c>
       <c r="F108" s="89">
-        <f t="shared" ref="F108:J108" ca="1" si="81">SUM(F104:F107)</f>
-        <v>126968.01850171364</v>
+        <f t="shared" ref="F108:J108" ca="1" si="83">SUM(F104:F107)</f>
+        <v>127762.1475374393</v>
       </c>
       <c r="G108" s="89">
-        <f t="shared" ca="1" si="81"/>
-        <v>134164.48209169364</v>
+        <f t="shared" ca="1" si="83"/>
+        <v>135864.17412696168</v>
       </c>
       <c r="H108" s="89">
-        <f t="shared" ca="1" si="81"/>
-        <v>142765.10532541786</v>
+        <f t="shared" ca="1" si="83"/>
+        <v>145414.49299432407</v>
       </c>
       <c r="I108" s="89">
-        <f t="shared" ca="1" si="81"/>
-        <v>152976.55550437322</v>
+        <f t="shared" ca="1" si="83"/>
+        <v>156626.68729367328</v>
       </c>
       <c r="J108" s="89">
-        <f t="shared" ca="1" si="81"/>
-        <v>165039.22880469891</v>
+        <f t="shared" ca="1" si="83"/>
+        <v>169739.16830634276</v>
       </c>
     </row>
     <row r="109" spans="2:10">
@@ -6617,24 +6647,24 @@
         <v>0</v>
       </c>
       <c r="F110" s="96">
-        <f t="shared" ref="F110:J110" ca="1" si="82">F95-(F102+F108)</f>
-        <v>-151339.64274614383</v>
+        <f t="shared" ref="F110:J110" ca="1" si="84">F95-(F102+F108)</f>
+        <v>0</v>
       </c>
       <c r="G110" s="96">
-        <f t="shared" ca="1" si="82"/>
-        <v>-158822.07608202755</v>
+        <f t="shared" ca="1" si="84"/>
+        <v>0</v>
       </c>
       <c r="H110" s="96">
-        <f t="shared" ca="1" si="82"/>
-        <v>-164721.65920837983</v>
+        <f t="shared" ca="1" si="84"/>
+        <v>-6.4028427004814148E-10</v>
       </c>
       <c r="I110" s="96">
-        <f t="shared" ca="1" si="82"/>
-        <v>-174496.68527417741</v>
+        <f t="shared" ca="1" si="84"/>
+        <v>1.1175870895385742E-8</v>
       </c>
       <c r="J110" s="96">
-        <f t="shared" ca="1" si="82"/>
-        <v>-179610.84961238003</v>
+        <f t="shared" ca="1" si="84"/>
+        <v>-1.1158408597111702E-7</v>
       </c>
     </row>
     <row r="111" spans="2:10">
@@ -6778,31 +6808,31 @@
       </c>
       <c r="C120" s="80"/>
       <c r="D120" s="80">
-        <f t="shared" ref="D120:J121" si="83">D13</f>
+        <f t="shared" ref="D120:J121" si="85">D13</f>
         <v>2012</v>
       </c>
       <c r="E120" s="80">
-        <f t="shared" si="83"/>
+        <f t="shared" si="85"/>
         <v>2013</v>
       </c>
       <c r="F120" s="81">
-        <f t="shared" si="83"/>
+        <f t="shared" si="85"/>
         <v>2014</v>
       </c>
       <c r="G120" s="81">
-        <f t="shared" si="83"/>
+        <f t="shared" si="85"/>
         <v>2015</v>
       </c>
       <c r="H120" s="81">
-        <f t="shared" si="83"/>
+        <f t="shared" si="85"/>
         <v>2016</v>
       </c>
       <c r="I120" s="81">
-        <f t="shared" si="83"/>
+        <f t="shared" si="85"/>
         <v>2017</v>
       </c>
       <c r="J120" s="81">
-        <f t="shared" si="83"/>
+        <f t="shared" si="85"/>
         <v>2018</v>
       </c>
     </row>
@@ -6813,31 +6843,31 @@
       </c>
       <c r="C121" s="82"/>
       <c r="D121" s="82">
-        <f t="shared" si="83"/>
+        <f t="shared" si="85"/>
         <v>41181</v>
       </c>
       <c r="E121" s="82">
-        <f t="shared" si="83"/>
+        <f t="shared" si="85"/>
         <v>41545</v>
       </c>
       <c r="F121" s="82">
-        <f t="shared" si="83"/>
+        <f t="shared" si="85"/>
         <v>41912</v>
       </c>
       <c r="G121" s="82">
-        <f t="shared" si="83"/>
+        <f t="shared" si="85"/>
         <v>42277</v>
       </c>
       <c r="H121" s="82">
-        <f t="shared" si="83"/>
+        <f t="shared" si="85"/>
         <v>42643</v>
       </c>
       <c r="I121" s="82">
-        <f t="shared" si="83"/>
+        <f t="shared" si="85"/>
         <v>43008</v>
       </c>
       <c r="J121" s="82">
-        <f t="shared" si="83"/>
+        <f t="shared" si="85"/>
         <v>43373</v>
       </c>
     </row>
@@ -6863,23 +6893,23 @@
       <c r="D124" s="3"/>
       <c r="E124" s="110"/>
       <c r="F124" s="111">
-        <f t="shared" ref="F124:J124" si="84">E126</f>
+        <f t="shared" ref="F124:J124" si="86">E126</f>
         <v>13102</v>
       </c>
       <c r="G124" s="111">
-        <f t="shared" si="84"/>
+        <f t="shared" si="86"/>
         <v>13535.190578699998</v>
       </c>
       <c r="H124" s="111">
-        <f t="shared" si="84"/>
+        <f t="shared" si="86"/>
         <v>14329.049503419239</v>
       </c>
       <c r="I124" s="111">
-        <f t="shared" si="84"/>
+        <f t="shared" si="86"/>
         <v>14970.912446547813</v>
       </c>
       <c r="J124" s="111">
-        <f t="shared" si="84"/>
+        <f t="shared" si="86"/>
         <v>15707.246187902134</v>
       </c>
     </row>
@@ -6895,19 +6925,19 @@
         <v>433.19057869999779</v>
       </c>
       <c r="G125" s="101">
-        <f t="shared" ref="G125:J125" si="85">G126-G124</f>
+        <f t="shared" ref="G125:J125" si="87">G126-G124</f>
         <v>793.85892471924126</v>
       </c>
       <c r="H125" s="101">
-        <f t="shared" si="85"/>
+        <f t="shared" si="87"/>
         <v>641.86294312857353</v>
       </c>
       <c r="I125" s="101">
-        <f t="shared" si="85"/>
+        <f t="shared" si="87"/>
         <v>736.33374135432132</v>
       </c>
       <c r="J125" s="101">
-        <f t="shared" si="85"/>
+        <f t="shared" si="87"/>
         <v>846.22252630906041</v>
       </c>
     </row>
@@ -6929,19 +6959,19 @@
         <v>13535.190578699998</v>
       </c>
       <c r="G126" s="101">
-        <f t="shared" ref="G126:J126" si="86">IF(G128,(G128*G16), G124*(G16/F16))</f>
+        <f t="shared" ref="G126:J126" si="88">IF(G128,(G128*G16), G124*(G16/F16))</f>
         <v>14329.049503419239</v>
       </c>
       <c r="H126" s="101">
-        <f t="shared" si="86"/>
+        <f t="shared" si="88"/>
         <v>14970.912446547813</v>
       </c>
       <c r="I126" s="101">
-        <f t="shared" si="86"/>
+        <f t="shared" si="88"/>
         <v>15707.246187902134</v>
       </c>
       <c r="J126" s="101">
-        <f t="shared" si="86"/>
+        <f t="shared" si="88"/>
         <v>16553.468714211194</v>
       </c>
     </row>
@@ -6992,23 +7022,23 @@
         <v>27.980984143701363</v>
       </c>
       <c r="F129" s="107">
-        <f t="shared" ref="F129:J129" si="87">365*F128</f>
+        <f t="shared" ref="F129:J129" si="89">365*F128</f>
         <v>27.557499999999997</v>
       </c>
       <c r="G129" s="107">
-        <f t="shared" si="87"/>
+        <f t="shared" si="89"/>
         <v>27.74</v>
       </c>
       <c r="H129" s="107">
-        <f t="shared" si="87"/>
+        <f t="shared" si="89"/>
         <v>27.74</v>
       </c>
       <c r="I129" s="107">
-        <f t="shared" si="87"/>
+        <f t="shared" si="89"/>
         <v>27.74</v>
       </c>
       <c r="J129" s="107">
-        <f t="shared" si="87"/>
+        <f t="shared" si="89"/>
         <v>27.74</v>
       </c>
     </row>
@@ -7052,15 +7082,15 @@
         <v>1804.2140130335999</v>
       </c>
       <c r="H132" s="108">
-        <f t="shared" ref="H132:J132" si="88">G134</f>
+        <f t="shared" ref="H132:J132" si="90">G134</f>
         <v>1947.4309515897016</v>
       </c>
       <c r="I132" s="108">
-        <f t="shared" si="88"/>
+        <f t="shared" si="90"/>
         <v>2034.6651928998995</v>
       </c>
       <c r="J132" s="108">
-        <f t="shared" si="88"/>
+        <f t="shared" si="90"/>
         <v>2134.7387615110679</v>
       </c>
     </row>
@@ -7076,19 +7106,19 @@
         <v>40.21401303359994</v>
       </c>
       <c r="G133" s="72">
-        <f t="shared" ref="G133:J133" si="89">G134-G132</f>
+        <f t="shared" ref="G133:J133" si="91">G134-G132</f>
         <v>143.2169385561017</v>
       </c>
       <c r="H133" s="72">
-        <f t="shared" si="89"/>
+        <f t="shared" si="91"/>
         <v>87.234241310197831</v>
       </c>
       <c r="I133" s="72">
-        <f t="shared" si="89"/>
+        <f t="shared" si="91"/>
         <v>100.07356861116841</v>
       </c>
       <c r="J133" s="72">
-        <f t="shared" si="89"/>
+        <f t="shared" si="91"/>
         <v>115.00832202955644</v>
       </c>
     </row>
@@ -7114,15 +7144,15 @@
         <v>1947.4309515897016</v>
       </c>
       <c r="H134" s="72">
-        <f t="shared" ref="H134:J134" si="90">-(IF(H136,(H136*H17),(G134*(H16/G16))))</f>
+        <f t="shared" ref="H134:J134" si="92">-(IF(H136,(H136*H17),(G134*(H16/G16))))</f>
         <v>2034.6651928998995</v>
       </c>
       <c r="I134" s="72">
-        <f t="shared" si="90"/>
+        <f t="shared" si="92"/>
         <v>2134.7387615110679</v>
       </c>
       <c r="J134" s="72">
-        <f t="shared" si="90"/>
+        <f t="shared" si="92"/>
         <v>2249.7470835406243</v>
       </c>
     </row>
@@ -7172,31 +7202,31 @@
       </c>
       <c r="C137" s="105"/>
       <c r="D137" s="73">
-        <f t="shared" ref="D137:J137" si="91">-(D17/D134)</f>
+        <f t="shared" ref="D137:J137" si="93">-(D17/D134)</f>
         <v>111.05689001264223</v>
       </c>
       <c r="E137" s="73">
-        <f t="shared" si="91"/>
+        <f t="shared" si="93"/>
         <v>60.434240362811792</v>
       </c>
       <c r="F137" s="73">
-        <f t="shared" si="91"/>
+        <f t="shared" si="93"/>
         <v>62.499999999999993</v>
       </c>
       <c r="G137" s="73">
-        <f t="shared" si="91"/>
+        <f t="shared" si="93"/>
         <v>60.606060606060602</v>
       </c>
       <c r="H137" s="73">
-        <f t="shared" si="91"/>
+        <f t="shared" si="93"/>
         <v>60.606060606060602</v>
       </c>
       <c r="I137" s="73">
-        <f t="shared" si="91"/>
+        <f t="shared" si="93"/>
         <v>60.606060606060602</v>
       </c>
       <c r="J137" s="73">
-        <f t="shared" si="91"/>
+        <f t="shared" si="93"/>
         <v>60.606060606060602</v>
       </c>
     </row>
@@ -7236,19 +7266,19 @@
         <v>22367</v>
       </c>
       <c r="G140" s="108">
-        <f t="shared" ref="G140:J140" si="92">F142</f>
+        <f t="shared" ref="G140:J140" si="94">F142</f>
         <v>22890.965290363798</v>
       </c>
       <c r="H140" s="108">
-        <f t="shared" si="92"/>
+        <f t="shared" si="94"/>
         <v>24313.380365301728</v>
       </c>
       <c r="I140" s="108">
-        <f t="shared" si="92"/>
+        <f t="shared" si="94"/>
         <v>25402.486650750256</v>
       </c>
       <c r="J140" s="108">
-        <f t="shared" si="92"/>
+        <f t="shared" si="94"/>
         <v>26651.889992198783</v>
       </c>
     </row>
@@ -7264,19 +7294,19 @@
         <v>523.96529036379798</v>
       </c>
       <c r="G141" s="72">
-        <f t="shared" ref="G141:J141" si="93">G142-G140</f>
+        <f t="shared" ref="G141:J141" si="95">G142-G140</f>
         <v>1422.4150749379296</v>
       </c>
       <c r="H141" s="72">
-        <f t="shared" si="93"/>
+        <f t="shared" si="95"/>
         <v>1089.1062854485281</v>
       </c>
       <c r="I141" s="72">
-        <f t="shared" si="93"/>
+        <f t="shared" si="95"/>
         <v>1249.4033414485275</v>
       </c>
       <c r="J141" s="72">
-        <f t="shared" si="93"/>
+        <f t="shared" si="95"/>
         <v>1435.8614750356755</v>
       </c>
     </row>
@@ -7298,19 +7328,19 @@
         <v>22890.965290363798</v>
       </c>
       <c r="G142" s="72">
-        <f t="shared" ref="G142:J142" si="94">-IF(G144,(G144*G17),(F142*(G17/F17)))</f>
+        <f t="shared" ref="G142:J142" si="96">-IF(G144,(G144*G17),(F142*(G17/F17)))</f>
         <v>24313.380365301728</v>
       </c>
       <c r="H142" s="72">
-        <f t="shared" si="94"/>
+        <f t="shared" si="96"/>
         <v>25402.486650750256</v>
       </c>
       <c r="I142" s="72">
-        <f t="shared" si="94"/>
+        <f t="shared" si="96"/>
         <v>26651.889992198783</v>
       </c>
       <c r="J142" s="72">
-        <f t="shared" si="94"/>
+        <f t="shared" si="96"/>
         <v>28087.751467234459</v>
       </c>
     </row>
@@ -7368,23 +7398,23 @@
         <v>76.580633360223629</v>
       </c>
       <c r="F145" s="71">
-        <f t="shared" ref="F145:J145" si="95">365*F144</f>
+        <f t="shared" ref="F145:J145" si="97">365*F144</f>
         <v>74.094999999999999</v>
       </c>
       <c r="G145" s="71">
-        <f t="shared" si="95"/>
+        <f t="shared" si="97"/>
         <v>75.19</v>
       </c>
       <c r="H145" s="71">
-        <f t="shared" si="95"/>
+        <f t="shared" si="97"/>
         <v>75.19</v>
       </c>
       <c r="I145" s="71">
-        <f t="shared" si="95"/>
+        <f t="shared" si="97"/>
         <v>75.19</v>
       </c>
       <c r="J145" s="71">
-        <f t="shared" si="95"/>
+        <f t="shared" si="97"/>
         <v>75.19</v>
       </c>
     </row>
@@ -7424,19 +7454,19 @@
         <v>23916</v>
       </c>
       <c r="G148" s="108">
-        <f t="shared" ref="G148:J148" si="96">F150</f>
+        <f t="shared" ref="G148:J148" si="98">F150</f>
         <v>23843.448304199999</v>
       </c>
       <c r="H148" s="108">
-        <f t="shared" si="96"/>
+        <f t="shared" si="98"/>
         <v>23850.325818191232</v>
       </c>
       <c r="I148" s="108">
-        <f t="shared" si="96"/>
+        <f t="shared" si="98"/>
         <v>23835.268500424805</v>
       </c>
       <c r="J148" s="108">
-        <f t="shared" si="96"/>
+        <f t="shared" si="98"/>
         <v>23974.217865745366</v>
       </c>
     </row>
@@ -7452,19 +7482,19 @@
         <v>-72.551695800000743</v>
       </c>
       <c r="G149" s="72">
-        <f t="shared" ref="G149:J149" si="97">G150-G148</f>
+        <f t="shared" ref="G149:J149" si="99">G150-G148</f>
         <v>6.8775139912322629</v>
       </c>
       <c r="H149" s="72">
-        <f t="shared" si="97"/>
+        <f t="shared" si="99"/>
         <v>-15.057317766426422</v>
       </c>
       <c r="I149" s="72">
-        <f t="shared" si="97"/>
+        <f t="shared" si="99"/>
         <v>138.9493653205609</v>
       </c>
       <c r="J149" s="72">
-        <f t="shared" si="97"/>
+        <f t="shared" si="99"/>
         <v>-15.249989913376339</v>
       </c>
     </row>
@@ -7486,19 +7516,19 @@
         <v>23843.448304199999</v>
       </c>
       <c r="G150" s="72">
-        <f t="shared" ref="G150:J150" si="98">IF(G152, (G16*G152), (F150*(G16/F16)))</f>
+        <f t="shared" ref="G150:J150" si="100">IF(G152, (G16*G152), (F150*(G16/F16)))</f>
         <v>23850.325818191232</v>
       </c>
       <c r="H150" s="72">
-        <f t="shared" si="98"/>
+        <f t="shared" si="100"/>
         <v>23835.268500424805</v>
       </c>
       <c r="I150" s="72">
-        <f t="shared" si="98"/>
+        <f t="shared" si="100"/>
         <v>23974.217865745366</v>
       </c>
       <c r="J150" s="72">
-        <f t="shared" si="98"/>
+        <f t="shared" si="100"/>
         <v>23958.96787583199</v>
       </c>
     </row>
@@ -7560,77 +7590,77 @@
     </row>
     <row r="155" spans="1:10">
       <c r="B155" s="79" t="str">
-        <f t="shared" ref="B155:J156" si="99">B13</f>
+        <f t="shared" ref="B155:J156" si="101">B13</f>
         <v xml:space="preserve">Fiscal year  </v>
       </c>
       <c r="C155" s="80">
-        <f t="shared" si="99"/>
+        <f t="shared" si="101"/>
         <v>2011</v>
       </c>
       <c r="D155" s="80">
-        <f t="shared" si="99"/>
+        <f t="shared" si="101"/>
         <v>2012</v>
       </c>
       <c r="E155" s="80">
-        <f t="shared" si="99"/>
+        <f t="shared" si="101"/>
         <v>2013</v>
       </c>
       <c r="F155" s="81">
-        <f t="shared" si="99"/>
+        <f t="shared" si="101"/>
         <v>2014</v>
       </c>
       <c r="G155" s="81">
-        <f t="shared" si="99"/>
+        <f t="shared" si="101"/>
         <v>2015</v>
       </c>
       <c r="H155" s="81">
-        <f t="shared" si="99"/>
+        <f t="shared" si="101"/>
         <v>2016</v>
       </c>
       <c r="I155" s="81">
-        <f t="shared" si="99"/>
+        <f t="shared" si="101"/>
         <v>2017</v>
       </c>
       <c r="J155" s="81">
-        <f t="shared" si="99"/>
+        <f t="shared" si="101"/>
         <v>2018</v>
       </c>
     </row>
     <row r="156" spans="1:10">
       <c r="B156" s="2" t="str">
-        <f t="shared" si="99"/>
+        <f t="shared" si="101"/>
         <v>Fiscal year end date</v>
       </c>
       <c r="C156" s="82">
-        <f t="shared" si="99"/>
+        <f t="shared" si="101"/>
         <v>40810</v>
       </c>
       <c r="D156" s="82">
-        <f t="shared" si="99"/>
+        <f t="shared" si="101"/>
         <v>41181</v>
       </c>
       <c r="E156" s="82">
-        <f t="shared" si="99"/>
+        <f t="shared" si="101"/>
         <v>41545</v>
       </c>
       <c r="F156" s="82">
-        <f t="shared" si="99"/>
+        <f t="shared" si="101"/>
         <v>41912</v>
       </c>
       <c r="G156" s="82">
-        <f t="shared" si="99"/>
+        <f t="shared" si="101"/>
         <v>42277</v>
       </c>
       <c r="H156" s="82">
-        <f t="shared" si="99"/>
+        <f t="shared" si="101"/>
         <v>42643</v>
       </c>
       <c r="I156" s="82">
-        <f t="shared" si="99"/>
+        <f t="shared" si="101"/>
         <v>43008</v>
       </c>
       <c r="J156" s="82">
-        <f t="shared" si="99"/>
+        <f t="shared" si="101"/>
         <v>43373</v>
       </c>
     </row>
@@ -7649,19 +7679,19 @@
         <v>5756</v>
       </c>
       <c r="G158" s="72">
-        <f t="shared" ref="G158:J158" si="100">F161</f>
+        <f t="shared" ref="G158:J158" si="102">F161</f>
         <v>4706</v>
       </c>
       <c r="H158" s="72">
-        <f t="shared" si="100"/>
+        <f t="shared" si="102"/>
         <v>3721</v>
       </c>
       <c r="I158" s="72">
-        <f t="shared" si="100"/>
+        <f t="shared" si="102"/>
         <v>2888</v>
       </c>
       <c r="J158" s="72">
-        <f t="shared" si="100"/>
+        <f t="shared" si="102"/>
         <v>2282</v>
       </c>
     </row>
@@ -7677,19 +7707,19 @@
         <v>0</v>
       </c>
       <c r="G159" s="68">
-        <f t="shared" ref="G159:J159" si="101">G163</f>
+        <f t="shared" ref="G159:J159" si="103">G163</f>
         <v>0</v>
       </c>
       <c r="H159" s="68">
-        <f t="shared" si="101"/>
+        <f t="shared" si="103"/>
         <v>0</v>
       </c>
       <c r="I159" s="68">
-        <f t="shared" si="101"/>
+        <f t="shared" si="103"/>
         <v>0</v>
       </c>
       <c r="J159" s="68">
-        <f t="shared" si="101"/>
+        <f t="shared" si="103"/>
         <v>0</v>
       </c>
     </row>
@@ -7705,19 +7735,19 @@
         <v>-1050</v>
       </c>
       <c r="G160" s="72">
-        <f t="shared" ref="G160:J160" si="102">G164</f>
+        <f t="shared" ref="G160:J160" si="104">G164</f>
         <v>-985</v>
       </c>
       <c r="H160" s="72">
-        <f t="shared" si="102"/>
+        <f t="shared" si="104"/>
         <v>-833</v>
       </c>
       <c r="I160" s="72">
-        <f t="shared" si="102"/>
+        <f t="shared" si="104"/>
         <v>-606</v>
       </c>
       <c r="J160" s="72">
-        <f t="shared" si="102"/>
+        <f t="shared" si="104"/>
         <v>-434</v>
       </c>
     </row>
@@ -7739,19 +7769,19 @@
         <v>4706</v>
       </c>
       <c r="G161" s="72">
-        <f t="shared" ref="G161:J161" si="103">SUM(G158:G160)</f>
+        <f t="shared" ref="G161:J161" si="105">SUM(G158:G160)</f>
         <v>3721</v>
       </c>
       <c r="H161" s="72">
-        <f t="shared" si="103"/>
+        <f t="shared" si="105"/>
         <v>2888</v>
       </c>
       <c r="I161" s="72">
-        <f t="shared" si="103"/>
+        <f t="shared" si="105"/>
         <v>2282</v>
       </c>
       <c r="J161" s="72">
-        <f t="shared" si="103"/>
+        <f t="shared" si="105"/>
         <v>1848</v>
       </c>
     </row>
@@ -7845,77 +7875,77 @@
     </row>
     <row r="167" spans="1:10">
       <c r="B167" s="79" t="str">
-        <f t="shared" ref="B167:J168" si="104">B13</f>
+        <f t="shared" ref="B167:J168" si="106">B13</f>
         <v xml:space="preserve">Fiscal year  </v>
       </c>
       <c r="C167" s="80">
-        <f t="shared" si="104"/>
+        <f t="shared" si="106"/>
         <v>2011</v>
       </c>
       <c r="D167" s="80">
-        <f t="shared" si="104"/>
+        <f t="shared" si="106"/>
         <v>2012</v>
       </c>
       <c r="E167" s="80">
-        <f t="shared" si="104"/>
+        <f t="shared" si="106"/>
         <v>2013</v>
       </c>
       <c r="F167" s="81">
-        <f t="shared" si="104"/>
+        <f t="shared" si="106"/>
         <v>2014</v>
       </c>
       <c r="G167" s="81">
-        <f t="shared" si="104"/>
+        <f t="shared" si="106"/>
         <v>2015</v>
       </c>
       <c r="H167" s="81">
-        <f t="shared" si="104"/>
+        <f t="shared" si="106"/>
         <v>2016</v>
       </c>
       <c r="I167" s="81">
-        <f t="shared" si="104"/>
+        <f t="shared" si="106"/>
         <v>2017</v>
       </c>
       <c r="J167" s="81">
-        <f t="shared" si="104"/>
+        <f t="shared" si="106"/>
         <v>2018</v>
       </c>
     </row>
     <row r="168" spans="1:10">
       <c r="B168" s="2" t="str">
-        <f t="shared" si="104"/>
+        <f t="shared" si="106"/>
         <v>Fiscal year end date</v>
       </c>
       <c r="C168" s="82">
-        <f t="shared" si="104"/>
+        <f t="shared" si="106"/>
         <v>40810</v>
       </c>
       <c r="D168" s="82">
-        <f t="shared" si="104"/>
+        <f t="shared" si="106"/>
         <v>41181</v>
       </c>
       <c r="E168" s="82">
-        <f t="shared" si="104"/>
+        <f t="shared" si="106"/>
         <v>41545</v>
       </c>
       <c r="F168" s="82">
-        <f t="shared" si="104"/>
+        <f t="shared" si="106"/>
         <v>41912</v>
       </c>
       <c r="G168" s="82">
-        <f t="shared" si="104"/>
+        <f t="shared" si="106"/>
         <v>42277</v>
       </c>
       <c r="H168" s="82">
-        <f t="shared" si="104"/>
+        <f t="shared" si="106"/>
         <v>42643</v>
       </c>
       <c r="I168" s="82">
-        <f t="shared" si="104"/>
+        <f t="shared" si="106"/>
         <v>43008</v>
       </c>
       <c r="J168" s="82">
-        <f t="shared" si="104"/>
+        <f t="shared" si="106"/>
         <v>43373</v>
       </c>
     </row>
@@ -7934,19 +7964,19 @@
         <v>16597</v>
       </c>
       <c r="G170" s="72">
-        <f t="shared" ref="G170:J170" si="105">F173</f>
+        <f t="shared" ref="G170:J170" si="107">F173</f>
         <v>19465.3847584</v>
       </c>
       <c r="H170" s="72">
-        <f t="shared" si="105"/>
+        <f t="shared" si="107"/>
         <v>23656.631738150129</v>
       </c>
       <c r="I170" s="72">
-        <f t="shared" si="105"/>
+        <f t="shared" si="107"/>
         <v>28035.623628765366</v>
       </c>
       <c r="J170" s="72">
-        <f t="shared" si="105"/>
+        <f t="shared" si="107"/>
         <v>32629.993138726739</v>
       </c>
     </row>
@@ -7962,19 +7992,19 @@
         <v>8963.7023699999991</v>
       </c>
       <c r="G171" s="72">
-        <f t="shared" ref="G171:J171" si="106">G175</f>
+        <f t="shared" ref="G171:J171" si="108">G175</f>
         <v>10746.78712756443</v>
       </c>
       <c r="H171" s="72">
-        <f t="shared" si="106"/>
+        <f t="shared" si="108"/>
         <v>11228.18433491086</v>
       </c>
       <c r="I171" s="72">
-        <f t="shared" si="106"/>
+        <f t="shared" si="108"/>
         <v>11780.434640926602</v>
       </c>
       <c r="J171" s="72">
-        <f t="shared" si="106"/>
+        <f t="shared" si="108"/>
         <v>12415.101535658396</v>
       </c>
     </row>
@@ -8030,19 +8060,19 @@
         <v>19465.3847584</v>
       </c>
       <c r="G173" s="72">
-        <f t="shared" ref="G173:J173" si="107">SUM(G170:G172)</f>
+        <f t="shared" ref="G173:J173" si="109">SUM(G170:G172)</f>
         <v>23656.631738150129</v>
       </c>
       <c r="H173" s="72">
-        <f t="shared" si="107"/>
+        <f t="shared" si="109"/>
         <v>28035.623628765366</v>
       </c>
       <c r="I173" s="72">
-        <f t="shared" si="107"/>
+        <f t="shared" si="109"/>
         <v>32629.993138726739</v>
       </c>
       <c r="J173" s="72">
-        <f t="shared" si="107"/>
+        <f t="shared" si="109"/>
         <v>37471.882737633518</v>
       </c>
     </row>
@@ -8075,19 +8105,19 @@
         <v>8963.7023699999991</v>
       </c>
       <c r="G175" s="72">
-        <f t="shared" ref="G175:J175" si="108">IF(G176,G176*G16,(F175*(G16/F16)))</f>
+        <f t="shared" ref="G175:J175" si="110">IF(G176,G176*G16,(F175*(G16/F16)))</f>
         <v>10746.78712756443</v>
       </c>
       <c r="H175" s="72">
-        <f t="shared" si="108"/>
+        <f t="shared" si="110"/>
         <v>11228.18433491086</v>
       </c>
       <c r="I175" s="72">
-        <f t="shared" si="108"/>
+        <f t="shared" si="110"/>
         <v>11780.434640926602</v>
       </c>
       <c r="J175" s="72">
-        <f t="shared" si="108"/>
+        <f t="shared" si="110"/>
         <v>12415.101535658396</v>
       </c>
     </row>
@@ -8100,11 +8130,11 @@
         <v>3.9353712274478286E-2</v>
       </c>
       <c r="D176" s="65">
-        <f t="shared" ref="D176:E176" si="109">D175/D16</f>
+        <f t="shared" ref="D176:E176" si="111">D175/D16</f>
         <v>5.3000485598180283E-2</v>
       </c>
       <c r="E176" s="65">
-        <f t="shared" si="109"/>
+        <f t="shared" si="111"/>
         <v>4.7773682054882687E-2</v>
       </c>
       <c r="F176" s="69">
@@ -8144,19 +8174,19 @@
         <v>-6095.3176115999995</v>
       </c>
       <c r="G177" s="72">
-        <f t="shared" ref="G177:J177" si="110">-(G178*G175)</f>
+        <f t="shared" ref="G177:J177" si="112">-(G178*G175)</f>
         <v>-6555.5401478143021</v>
       </c>
       <c r="H177" s="72">
-        <f t="shared" si="110"/>
+        <f t="shared" si="112"/>
         <v>-6849.1924442956242</v>
       </c>
       <c r="I177" s="72">
-        <f t="shared" si="110"/>
+        <f t="shared" si="112"/>
         <v>-7186.0651309652267</v>
       </c>
       <c r="J177" s="72">
-        <f t="shared" si="110"/>
+        <f t="shared" si="112"/>
         <v>-7573.2119367516216</v>
       </c>
     </row>
@@ -8210,77 +8240,77 @@
     </row>
     <row r="181" spans="1:10">
       <c r="B181" s="79" t="str">
-        <f t="shared" ref="B181:J182" si="111">B13</f>
+        <f t="shared" ref="B181:J182" si="113">B13</f>
         <v xml:space="preserve">Fiscal year  </v>
       </c>
       <c r="C181" s="80">
-        <f t="shared" si="111"/>
+        <f t="shared" si="113"/>
         <v>2011</v>
       </c>
       <c r="D181" s="80">
-        <f t="shared" si="111"/>
+        <f t="shared" si="113"/>
         <v>2012</v>
       </c>
       <c r="E181" s="80">
-        <f t="shared" si="111"/>
+        <f t="shared" si="113"/>
         <v>2013</v>
       </c>
       <c r="F181" s="81">
-        <f t="shared" si="111"/>
+        <f t="shared" si="113"/>
         <v>2014</v>
       </c>
       <c r="G181" s="81">
-        <f t="shared" si="111"/>
+        <f t="shared" si="113"/>
         <v>2015</v>
       </c>
       <c r="H181" s="81">
-        <f t="shared" si="111"/>
+        <f t="shared" si="113"/>
         <v>2016</v>
       </c>
       <c r="I181" s="81">
-        <f t="shared" si="111"/>
+        <f t="shared" si="113"/>
         <v>2017</v>
       </c>
       <c r="J181" s="81">
-        <f t="shared" si="111"/>
+        <f t="shared" si="113"/>
         <v>2018</v>
       </c>
     </row>
     <row r="182" spans="1:10">
       <c r="B182" s="2" t="str">
-        <f t="shared" si="111"/>
+        <f t="shared" si="113"/>
         <v>Fiscal year end date</v>
       </c>
       <c r="C182" s="82">
-        <f t="shared" si="111"/>
+        <f t="shared" si="113"/>
         <v>40810</v>
       </c>
       <c r="D182" s="82">
-        <f t="shared" si="111"/>
+        <f t="shared" si="113"/>
         <v>41181</v>
       </c>
       <c r="E182" s="82">
-        <f t="shared" si="111"/>
+        <f t="shared" si="113"/>
         <v>41545</v>
       </c>
       <c r="F182" s="82">
-        <f t="shared" si="111"/>
+        <f t="shared" si="113"/>
         <v>41912</v>
       </c>
       <c r="G182" s="82">
-        <f t="shared" si="111"/>
+        <f t="shared" si="113"/>
         <v>42277</v>
       </c>
       <c r="H182" s="82">
-        <f t="shared" si="111"/>
+        <f t="shared" si="113"/>
         <v>42643</v>
       </c>
       <c r="I182" s="82">
-        <f t="shared" si="111"/>
+        <f t="shared" si="113"/>
         <v>43008</v>
       </c>
       <c r="J182" s="82">
-        <f t="shared" si="111"/>
+        <f t="shared" si="113"/>
         <v>43373</v>
       </c>
     </row>
@@ -8303,19 +8333,19 @@
         <v>14421</v>
       </c>
       <c r="G185" s="72">
-        <f t="shared" ref="G185:J185" si="112">F187</f>
+        <f t="shared" ref="G185:J185" si="114">F187</f>
         <v>14421</v>
       </c>
       <c r="H185" s="72">
-        <f t="shared" si="112"/>
+        <f t="shared" si="114"/>
         <v>14421</v>
       </c>
       <c r="I185" s="72">
-        <f t="shared" si="112"/>
+        <f t="shared" si="114"/>
         <v>14421</v>
       </c>
       <c r="J185" s="72">
-        <f t="shared" si="112"/>
+        <f t="shared" si="114"/>
         <v>14421</v>
       </c>
     </row>
@@ -8358,19 +8388,19 @@
         <v>14421</v>
       </c>
       <c r="G187" s="72">
-        <f t="shared" ref="G187:J187" si="113">SUM(G185:G186)</f>
+        <f t="shared" ref="G187:J187" si="115">SUM(G185:G186)</f>
         <v>14421</v>
       </c>
       <c r="H187" s="72">
-        <f t="shared" si="113"/>
+        <f t="shared" si="115"/>
         <v>14421</v>
       </c>
       <c r="I187" s="72">
-        <f t="shared" si="113"/>
+        <f t="shared" si="115"/>
         <v>14421</v>
       </c>
       <c r="J187" s="72">
-        <f t="shared" si="113"/>
+        <f t="shared" si="115"/>
         <v>14421</v>
       </c>
     </row>
@@ -8407,19 +8437,19 @@
         <v>3453</v>
       </c>
       <c r="G190" s="72">
-        <f t="shared" ref="G190:J190" si="114">F192</f>
+        <f t="shared" ref="G190:J190" si="116">F192</f>
         <v>3453</v>
       </c>
       <c r="H190" s="72">
-        <f t="shared" si="114"/>
+        <f t="shared" si="116"/>
         <v>3453</v>
       </c>
       <c r="I190" s="72">
-        <f t="shared" si="114"/>
+        <f t="shared" si="116"/>
         <v>3453</v>
       </c>
       <c r="J190" s="72">
-        <f t="shared" si="114"/>
+        <f t="shared" si="116"/>
         <v>3453</v>
       </c>
     </row>
@@ -8462,19 +8492,19 @@
         <v>3453</v>
       </c>
       <c r="G192" s="72">
-        <f t="shared" ref="G192:J192" si="115">SUM(G190:G191)</f>
+        <f t="shared" ref="G192:J192" si="117">SUM(G190:G191)</f>
         <v>3453</v>
       </c>
       <c r="H192" s="72">
-        <f t="shared" si="115"/>
+        <f t="shared" si="117"/>
         <v>3453</v>
       </c>
       <c r="I192" s="72">
-        <f t="shared" si="115"/>
+        <f t="shared" si="117"/>
         <v>3453</v>
       </c>
       <c r="J192" s="72">
-        <f t="shared" si="115"/>
+        <f t="shared" si="117"/>
         <v>3453</v>
       </c>
     </row>
@@ -8511,19 +8541,19 @@
         <v>5146</v>
       </c>
       <c r="G195" s="72">
-        <f t="shared" ref="G195:J195" si="116">F197</f>
+        <f t="shared" ref="G195:J195" si="118">F197</f>
         <v>5146</v>
       </c>
       <c r="H195" s="72">
-        <f t="shared" si="116"/>
+        <f t="shared" si="118"/>
         <v>5146</v>
       </c>
       <c r="I195" s="72">
-        <f t="shared" si="116"/>
+        <f t="shared" si="118"/>
         <v>5146</v>
       </c>
       <c r="J195" s="72">
-        <f t="shared" si="116"/>
+        <f t="shared" si="118"/>
         <v>5146</v>
       </c>
     </row>
@@ -8566,19 +8596,19 @@
         <v>5146</v>
       </c>
       <c r="G197" s="72">
-        <f t="shared" ref="G197:J197" si="117">SUM(G195:G196)</f>
+        <f t="shared" ref="G197:J197" si="119">SUM(G195:G196)</f>
         <v>5146</v>
       </c>
       <c r="H197" s="72">
-        <f t="shared" si="117"/>
+        <f t="shared" si="119"/>
         <v>5146</v>
       </c>
       <c r="I197" s="72">
-        <f t="shared" si="117"/>
+        <f t="shared" si="119"/>
         <v>5146</v>
       </c>
       <c r="J197" s="72">
-        <f t="shared" si="117"/>
+        <f t="shared" si="119"/>
         <v>5146</v>
       </c>
     </row>
@@ -8615,19 +8645,19 @@
         <v>20208</v>
       </c>
       <c r="G200" s="72">
-        <f t="shared" ref="G200:J200" si="118">F202</f>
+        <f t="shared" ref="G200:J200" si="120">F202</f>
         <v>23208</v>
       </c>
       <c r="H200" s="72">
-        <f t="shared" si="118"/>
+        <f t="shared" si="120"/>
         <v>26208</v>
       </c>
       <c r="I200" s="72">
-        <f t="shared" si="118"/>
+        <f t="shared" si="120"/>
         <v>29208</v>
       </c>
       <c r="J200" s="72">
-        <f t="shared" si="118"/>
+        <f t="shared" si="120"/>
         <v>32208</v>
       </c>
     </row>
@@ -8675,15 +8705,15 @@
         <v>26208</v>
       </c>
       <c r="H202" s="72">
-        <f t="shared" ref="G202:J202" si="119">SUM(H200:H201)</f>
+        <f t="shared" ref="G202:J202" si="121">SUM(H200:H201)</f>
         <v>29208</v>
       </c>
       <c r="I202" s="72">
-        <f t="shared" si="119"/>
+        <f t="shared" si="121"/>
         <v>32208</v>
       </c>
       <c r="J202" s="72">
-        <f t="shared" si="119"/>
+        <f t="shared" si="121"/>
         <v>35208</v>
       </c>
     </row>
@@ -8710,31 +8740,31 @@
       </c>
       <c r="C205" s="80"/>
       <c r="D205" s="80">
-        <f t="shared" ref="D205:J206" si="120">D13</f>
+        <f t="shared" ref="D205:J206" si="122">D13</f>
         <v>2012</v>
       </c>
       <c r="E205" s="80">
-        <f t="shared" si="120"/>
+        <f t="shared" si="122"/>
         <v>2013</v>
       </c>
       <c r="F205" s="81">
-        <f t="shared" si="120"/>
+        <f t="shared" si="122"/>
         <v>2014</v>
       </c>
       <c r="G205" s="81">
-        <f t="shared" si="120"/>
+        <f t="shared" si="122"/>
         <v>2015</v>
       </c>
       <c r="H205" s="81">
-        <f t="shared" si="120"/>
+        <f t="shared" si="122"/>
         <v>2016</v>
       </c>
       <c r="I205" s="81">
-        <f t="shared" si="120"/>
+        <f t="shared" si="122"/>
         <v>2017</v>
       </c>
       <c r="J205" s="81">
-        <f t="shared" si="120"/>
+        <f t="shared" si="122"/>
         <v>2018</v>
       </c>
     </row>
@@ -8745,31 +8775,31 @@
       </c>
       <c r="C206" s="82"/>
       <c r="D206" s="82">
-        <f t="shared" si="120"/>
+        <f t="shared" si="122"/>
         <v>41181</v>
       </c>
       <c r="E206" s="82">
-        <f t="shared" si="120"/>
+        <f t="shared" si="122"/>
         <v>41545</v>
       </c>
       <c r="F206" s="82">
-        <f t="shared" si="120"/>
+        <f t="shared" si="122"/>
         <v>41912</v>
       </c>
       <c r="G206" s="82">
-        <f t="shared" si="120"/>
+        <f t="shared" si="122"/>
         <v>42277</v>
       </c>
       <c r="H206" s="82">
-        <f t="shared" si="120"/>
+        <f t="shared" si="122"/>
         <v>42643</v>
       </c>
       <c r="I206" s="82">
-        <f t="shared" si="120"/>
+        <f t="shared" si="122"/>
         <v>43008</v>
       </c>
       <c r="J206" s="82">
-        <f t="shared" si="120"/>
+        <f t="shared" si="122"/>
         <v>43373</v>
       </c>
     </row>
@@ -8792,19 +8822,19 @@
         <v>16960</v>
       </c>
       <c r="G209" s="96">
-        <f t="shared" ref="G209:J209" si="121">F212</f>
+        <f t="shared" ref="G209:J209" si="123">F212</f>
         <v>16960</v>
       </c>
       <c r="H209" s="96">
-        <f t="shared" si="121"/>
+        <f t="shared" si="123"/>
         <v>16960</v>
       </c>
       <c r="I209" s="96">
-        <f t="shared" si="121"/>
+        <f t="shared" si="123"/>
         <v>14460</v>
       </c>
       <c r="J209" s="96">
-        <f t="shared" si="121"/>
+        <f t="shared" si="123"/>
         <v>14460</v>
       </c>
     </row>
@@ -8843,19 +8873,19 @@
         <v>0</v>
       </c>
       <c r="G211">
-        <f t="shared" ref="G211:J211" si="122">G214*G218</f>
+        <f t="shared" ref="G211:J211" si="124">G214*G218</f>
         <v>0</v>
       </c>
       <c r="H211">
-        <f t="shared" si="122"/>
+        <f t="shared" si="124"/>
         <v>0</v>
       </c>
       <c r="I211">
-        <f t="shared" si="122"/>
+        <f t="shared" si="124"/>
         <v>0</v>
       </c>
       <c r="J211">
-        <f t="shared" si="122"/>
+        <f t="shared" si="124"/>
         <v>0</v>
       </c>
     </row>
@@ -8876,19 +8906,19 @@
         <v>16960</v>
       </c>
       <c r="G212" s="96">
-        <f t="shared" ref="G212:J212" si="123">SUM(G209:G211)</f>
+        <f t="shared" ref="G212:J212" si="125">SUM(G209:G211)</f>
         <v>16960</v>
       </c>
       <c r="H212" s="96">
-        <f t="shared" si="123"/>
+        <f t="shared" si="125"/>
         <v>14460</v>
       </c>
       <c r="I212" s="96">
-        <f t="shared" si="123"/>
+        <f t="shared" si="125"/>
         <v>14460</v>
       </c>
       <c r="J212" s="96">
-        <f t="shared" si="123"/>
+        <f t="shared" si="125"/>
         <v>8460</v>
       </c>
     </row>
@@ -8921,7 +8951,7 @@
         <v>316.70000000000005</v>
       </c>
       <c r="I214" s="120">
-        <f t="shared" ref="I214:J214" si="124">0.011*2000+0.0108*4000+0.0244*5500+0.0391*3000</f>
+        <f t="shared" ref="I214:J214" si="126">0.011*2000+0.0108*4000+0.0244*5500+0.0391*3000</f>
         <v>316.70000000000005</v>
       </c>
       <c r="J214" s="120">
@@ -8940,19 +8970,19 @@
         <v>1.9425117924528303E-2</v>
       </c>
       <c r="G215" s="56">
-        <f t="shared" ref="G215:J215" si="125">G214/AVERAGE(G212,G209)</f>
+        <f t="shared" ref="G215:J215" si="127">G214/AVERAGE(G212,G209)</f>
         <v>1.9425117924528303E-2</v>
       </c>
       <c r="H215" s="56">
-        <f t="shared" si="125"/>
+        <f t="shared" si="127"/>
         <v>2.0159134309357101E-2</v>
       </c>
       <c r="I215" s="56">
-        <f t="shared" si="125"/>
+        <f t="shared" si="127"/>
         <v>2.1901798063623794E-2</v>
       </c>
       <c r="J215" s="56">
-        <f t="shared" si="125"/>
+        <f t="shared" si="127"/>
         <v>2.1945898778359514E-2</v>
       </c>
     </row>
@@ -8999,19 +9029,19 @@
         <v>0</v>
       </c>
       <c r="G218" s="121">
-        <f t="shared" ref="G218:J218" si="126">1-G217</f>
+        <f t="shared" ref="G218:J218" si="128">1-G217</f>
         <v>0</v>
       </c>
       <c r="H218" s="121">
-        <f t="shared" si="126"/>
+        <f t="shared" si="128"/>
         <v>0</v>
       </c>
       <c r="I218" s="121">
-        <f t="shared" si="126"/>
+        <f t="shared" si="128"/>
         <v>0</v>
       </c>
       <c r="J218" s="121">
-        <f t="shared" si="126"/>
+        <f t="shared" si="128"/>
         <v>0</v>
       </c>
     </row>
@@ -9033,71 +9063,71 @@
     </row>
     <row r="221" spans="1:10">
       <c r="B221" s="79" t="str">
-        <f t="shared" ref="B221:B222" si="127">B13</f>
+        <f t="shared" ref="B221:B222" si="129">B13</f>
         <v xml:space="preserve">Fiscal year  </v>
       </c>
       <c r="C221" s="80"/>
       <c r="D221" s="80">
-        <f t="shared" ref="D221:J222" si="128">D13</f>
+        <f t="shared" ref="D221:J222" si="130">D13</f>
         <v>2012</v>
       </c>
       <c r="E221" s="80">
-        <f t="shared" si="128"/>
+        <f t="shared" si="130"/>
         <v>2013</v>
       </c>
       <c r="F221" s="81">
-        <f t="shared" si="128"/>
+        <f t="shared" si="130"/>
         <v>2014</v>
       </c>
       <c r="G221" s="81">
-        <f t="shared" si="128"/>
+        <f t="shared" si="130"/>
         <v>2015</v>
       </c>
       <c r="H221" s="81">
-        <f t="shared" si="128"/>
+        <f t="shared" si="130"/>
         <v>2016</v>
       </c>
       <c r="I221" s="81">
-        <f t="shared" si="128"/>
+        <f t="shared" si="130"/>
         <v>2017</v>
       </c>
       <c r="J221" s="81">
-        <f t="shared" si="128"/>
+        <f t="shared" si="130"/>
         <v>2018</v>
       </c>
     </row>
     <row r="222" spans="1:10">
       <c r="B222" s="2" t="str">
-        <f t="shared" si="127"/>
+        <f t="shared" si="129"/>
         <v>Fiscal year end date</v>
       </c>
       <c r="C222" s="82"/>
       <c r="D222" s="82">
-        <f t="shared" si="128"/>
+        <f t="shared" si="130"/>
         <v>41181</v>
       </c>
       <c r="E222" s="82">
-        <f t="shared" si="128"/>
+        <f t="shared" si="130"/>
         <v>41545</v>
       </c>
       <c r="F222" s="82">
-        <f t="shared" si="128"/>
+        <f t="shared" si="130"/>
         <v>41912</v>
       </c>
       <c r="G222" s="82">
-        <f t="shared" si="128"/>
+        <f t="shared" si="130"/>
         <v>42277</v>
       </c>
       <c r="H222" s="82">
-        <f t="shared" si="128"/>
+        <f t="shared" si="130"/>
         <v>42643</v>
       </c>
       <c r="I222" s="82">
-        <f t="shared" si="128"/>
+        <f t="shared" si="130"/>
         <v>43008</v>
       </c>
       <c r="J222" s="82">
-        <f t="shared" si="128"/>
+        <f t="shared" si="130"/>
         <v>43373</v>
       </c>
     </row>
@@ -9121,19 +9151,19 @@
         <v>19764</v>
       </c>
       <c r="G225" s="72">
-        <f t="shared" ref="G225:J225" si="129">F228</f>
+        <f t="shared" ref="G225:J225" si="131">F228</f>
         <v>21976.600293010801</v>
       </c>
       <c r="H225" s="72">
-        <f t="shared" si="129"/>
+        <f t="shared" si="131"/>
         <v>24163.665743532685</v>
       </c>
       <c r="I225" s="72">
-        <f t="shared" si="129"/>
+        <f t="shared" si="131"/>
         <v>26448.69974853209</v>
       </c>
       <c r="J225" s="72">
-        <f t="shared" si="129"/>
+        <f t="shared" si="131"/>
         <v>28846.121535106628</v>
       </c>
     </row>
@@ -9149,19 +9179,19 @@
         <v>0</v>
       </c>
       <c r="G226" s="68">
-        <f t="shared" ref="G226:J226" si="130">G230</f>
+        <f t="shared" ref="G226:J226" si="132">G230</f>
         <v>0</v>
       </c>
       <c r="H226" s="68">
-        <f t="shared" si="130"/>
+        <f t="shared" si="132"/>
         <v>0</v>
       </c>
       <c r="I226" s="68">
-        <f t="shared" si="130"/>
+        <f t="shared" si="132"/>
         <v>0</v>
       </c>
       <c r="J226" s="68">
-        <f t="shared" si="130"/>
+        <f t="shared" si="132"/>
         <v>0</v>
       </c>
     </row>
@@ -9177,19 +9207,19 @@
         <v>2212.6002930107998</v>
       </c>
       <c r="G227" s="72">
-        <f t="shared" ref="G227:J227" si="131">G231</f>
+        <f t="shared" ref="G227:J227" si="133">G231</f>
         <v>2187.0654505218836</v>
       </c>
       <c r="H227" s="72">
-        <f t="shared" si="131"/>
+        <f t="shared" si="133"/>
         <v>2285.0340049994029</v>
       </c>
       <c r="I227" s="72">
-        <f t="shared" si="131"/>
+        <f t="shared" si="133"/>
         <v>2397.4217865745363</v>
       </c>
       <c r="J227" s="72">
-        <f t="shared" si="131"/>
+        <f t="shared" si="133"/>
         <v>2526.5820669059194</v>
       </c>
     </row>
@@ -9211,19 +9241,19 @@
         <v>21976.600293010801</v>
       </c>
       <c r="G228" s="72">
-        <f t="shared" ref="G228:J228" si="132">SUM(G225:G227)</f>
+        <f t="shared" ref="G228:J228" si="134">SUM(G225:G227)</f>
         <v>24163.665743532685</v>
       </c>
       <c r="H228" s="72">
-        <f t="shared" si="132"/>
+        <f t="shared" si="134"/>
         <v>26448.69974853209</v>
       </c>
       <c r="I228" s="72">
-        <f t="shared" si="132"/>
+        <f t="shared" si="134"/>
         <v>28846.121535106628</v>
       </c>
       <c r="J228" s="72">
-        <f t="shared" si="132"/>
+        <f t="shared" si="134"/>
         <v>31372.703602012545</v>
       </c>
     </row>
@@ -9281,19 +9311,19 @@
         <v>2212.6002930107998</v>
       </c>
       <c r="G231" s="72">
-        <f t="shared" ref="G231:J231" si="133">-(G232*SUM(G17,G19:G20))</f>
+        <f t="shared" ref="G231:J231" si="135">-(G232*SUM(G17,G19:G20))</f>
         <v>2187.0654505218836</v>
       </c>
       <c r="H231" s="72">
-        <f t="shared" si="133"/>
+        <f t="shared" si="135"/>
         <v>2285.0340049994029</v>
       </c>
       <c r="I231" s="72">
-        <f t="shared" si="133"/>
+        <f t="shared" si="135"/>
         <v>2397.4217865745363</v>
       </c>
       <c r="J231" s="72">
-        <f t="shared" si="133"/>
+        <f t="shared" si="135"/>
         <v>2526.5820669059194</v>
       </c>
     </row>
@@ -9362,19 +9392,19 @@
         <v>0</v>
       </c>
       <c r="G235" s="72">
-        <f t="shared" ref="G235:J235" si="134">F237</f>
+        <f t="shared" ref="G235:J235" si="136">F237</f>
         <v>-23968</v>
       </c>
       <c r="H235" s="72">
-        <f t="shared" si="134"/>
+        <f t="shared" si="136"/>
         <v>-47936</v>
       </c>
       <c r="I235" s="72">
-        <f t="shared" si="134"/>
+        <f t="shared" si="136"/>
         <v>-71904</v>
       </c>
       <c r="J235" s="72">
-        <f t="shared" si="134"/>
+        <f t="shared" si="136"/>
         <v>-95872</v>
       </c>
     </row>
@@ -9390,19 +9420,19 @@
         <v>-23968</v>
       </c>
       <c r="G236" s="72">
-        <f t="shared" ref="G236:J236" si="135">G239</f>
+        <f t="shared" ref="G236:J236" si="137">G239</f>
         <v>-23968</v>
       </c>
       <c r="H236" s="72">
-        <f t="shared" si="135"/>
+        <f t="shared" si="137"/>
         <v>-23968</v>
       </c>
       <c r="I236" s="72">
-        <f t="shared" si="135"/>
+        <f t="shared" si="137"/>
         <v>-23968</v>
       </c>
       <c r="J236" s="72">
-        <f t="shared" si="135"/>
+        <f t="shared" si="137"/>
         <v>-23968</v>
       </c>
     </row>
@@ -9424,19 +9454,19 @@
         <v>-23968</v>
       </c>
       <c r="G237" s="72">
-        <f t="shared" ref="G237:J237" si="136">SUM(G235:G236)</f>
+        <f t="shared" ref="G237:J237" si="138">SUM(G235:G236)</f>
         <v>-47936</v>
       </c>
       <c r="H237" s="72">
-        <f t="shared" si="136"/>
+        <f t="shared" si="138"/>
         <v>-71904</v>
       </c>
       <c r="I237" s="72">
-        <f t="shared" si="136"/>
+        <f t="shared" si="138"/>
         <v>-95872</v>
       </c>
       <c r="J237" s="72">
-        <f t="shared" si="136"/>
+        <f t="shared" si="138"/>
         <v>-119840</v>
       </c>
     </row>
@@ -9496,77 +9526,77 @@
     </row>
     <row r="242" spans="1:10">
       <c r="B242" s="79" t="str">
-        <f t="shared" ref="B242:J243" si="137">B13</f>
+        <f t="shared" ref="B242:J243" si="139">B13</f>
         <v xml:space="preserve">Fiscal year  </v>
       </c>
       <c r="C242" s="80">
-        <f t="shared" si="137"/>
+        <f t="shared" si="139"/>
         <v>2011</v>
       </c>
       <c r="D242" s="80">
-        <f t="shared" si="137"/>
+        <f t="shared" si="139"/>
         <v>2012</v>
       </c>
       <c r="E242" s="80">
-        <f t="shared" si="137"/>
+        <f t="shared" si="139"/>
         <v>2013</v>
       </c>
       <c r="F242" s="81">
-        <f t="shared" si="137"/>
+        <f t="shared" si="139"/>
         <v>2014</v>
       </c>
       <c r="G242" s="81">
-        <f t="shared" si="137"/>
+        <f t="shared" si="139"/>
         <v>2015</v>
       </c>
       <c r="H242" s="81">
-        <f t="shared" si="137"/>
+        <f t="shared" si="139"/>
         <v>2016</v>
       </c>
       <c r="I242" s="81">
-        <f t="shared" si="137"/>
+        <f t="shared" si="139"/>
         <v>2017</v>
       </c>
       <c r="J242" s="81">
-        <f t="shared" si="137"/>
+        <f t="shared" si="139"/>
         <v>2018</v>
       </c>
     </row>
     <row r="243" spans="1:10">
       <c r="B243" s="2" t="str">
-        <f t="shared" si="137"/>
+        <f t="shared" si="139"/>
         <v>Fiscal year end date</v>
       </c>
       <c r="C243" s="82">
-        <f t="shared" si="137"/>
+        <f t="shared" si="139"/>
         <v>40810</v>
       </c>
       <c r="D243" s="82">
-        <f t="shared" si="137"/>
+        <f t="shared" si="139"/>
         <v>41181</v>
       </c>
       <c r="E243" s="82">
-        <f t="shared" si="137"/>
+        <f t="shared" si="139"/>
         <v>41545</v>
       </c>
       <c r="F243" s="82">
-        <f t="shared" si="137"/>
+        <f t="shared" si="139"/>
         <v>41912</v>
       </c>
       <c r="G243" s="82">
-        <f t="shared" si="137"/>
+        <f t="shared" si="139"/>
         <v>42277</v>
       </c>
       <c r="H243" s="82">
-        <f t="shared" si="137"/>
+        <f t="shared" si="139"/>
         <v>42643</v>
       </c>
       <c r="I243" s="82">
-        <f t="shared" si="137"/>
+        <f t="shared" si="139"/>
         <v>43008</v>
       </c>
       <c r="J243" s="82">
-        <f t="shared" si="137"/>
+        <f t="shared" si="139"/>
         <v>43373</v>
       </c>
     </row>
@@ -9598,20 +9628,20 @@
         <v>104256</v>
       </c>
       <c r="G246" s="64">
-        <f t="shared" ref="G246:J246" ca="1" si="138">F249</f>
-        <v>129430.41820870283</v>
+        <f t="shared" ref="G246:J246" ca="1" si="140">F249</f>
+        <v>130224.54724442851</v>
       </c>
       <c r="H246" s="64">
-        <f t="shared" ca="1" si="138"/>
-        <v>158407.81634816097</v>
+        <f t="shared" ca="1" si="140"/>
+        <v>160107.508383429</v>
       </c>
       <c r="I246" s="64">
-        <f t="shared" ca="1" si="138"/>
-        <v>188691.40557688577</v>
+        <f t="shared" ca="1" si="140"/>
+        <v>191340.79324579198</v>
       </c>
       <c r="J246" s="64">
-        <f t="shared" ca="1" si="138"/>
-        <v>220473.4339692666</v>
+        <f t="shared" ca="1" si="140"/>
+        <v>224123.56575856666</v>
       </c>
     </row>
     <row r="247" spans="1:10">
@@ -9623,23 +9653,23 @@
       <c r="E247"/>
       <c r="F247" s="64">
         <f ca="1">F251</f>
-        <v>35963.454583861196</v>
+        <v>37097.92463489787</v>
       </c>
       <c r="G247" s="64">
-        <f t="shared" ref="G247:J247" ca="1" si="139">G251</f>
-        <v>38128.155446655452</v>
+        <f t="shared" ref="G247:J247" ca="1" si="141">G251</f>
+        <v>39319.685709211175</v>
       </c>
       <c r="H247" s="64">
-        <f t="shared" ca="1" si="139"/>
-        <v>39846.827932532637</v>
+        <f t="shared" ca="1" si="141"/>
+        <v>41096.427450476906</v>
       </c>
       <c r="I247" s="64">
-        <f t="shared" ca="1" si="139"/>
-        <v>41818.458411027415</v>
+        <f t="shared" ca="1" si="141"/>
+        <v>43135.226990506402</v>
       </c>
       <c r="J247" s="64">
-        <f t="shared" ca="1" si="139"/>
-        <v>44084.330570289167</v>
+        <f t="shared" ca="1" si="141"/>
+        <v>45465.656507429085</v>
       </c>
     </row>
     <row r="248" spans="1:10">
@@ -9651,23 +9681,23 @@
       <c r="E248"/>
       <c r="F248" s="72">
         <f ca="1">(F253)</f>
-        <v>-10789.036375158359</v>
+        <v>-11129.377390469361</v>
       </c>
       <c r="G248" s="72">
-        <f t="shared" ref="G248:J248" ca="1" si="140">(G253)</f>
-        <v>-9150.7573071973075</v>
+        <f t="shared" ref="G248:J248" ca="1" si="142">(G253)</f>
+        <v>-9436.7245702106811</v>
       </c>
       <c r="H248" s="72">
-        <f t="shared" ca="1" si="140"/>
-        <v>-9563.2387038078323</v>
+        <f t="shared" ca="1" si="142"/>
+        <v>-9863.1425881144569</v>
       </c>
       <c r="I248" s="72">
-        <f t="shared" ca="1" si="140"/>
-        <v>-10036.430018646579</v>
+        <f t="shared" ca="1" si="142"/>
+        <v>-10352.454477721536</v>
       </c>
       <c r="J248" s="72">
-        <f t="shared" ca="1" si="140"/>
-        <v>-10580.239336869399</v>
+        <f t="shared" ca="1" si="142"/>
+        <v>-10911.757561782981</v>
       </c>
     </row>
     <row r="249" spans="1:10">
@@ -9683,23 +9713,23 @@
       </c>
       <c r="F249" s="64">
         <f ca="1">SUM(F246:F248)</f>
-        <v>129430.41820870283</v>
+        <v>130224.54724442851</v>
       </c>
       <c r="G249" s="64">
-        <f t="shared" ref="G249:J249" ca="1" si="141">SUM(G246:G248)</f>
-        <v>158407.81634816097</v>
+        <f t="shared" ref="G249:J249" ca="1" si="143">SUM(G246:G248)</f>
+        <v>160107.50838342903</v>
       </c>
       <c r="H249" s="64">
-        <f t="shared" ca="1" si="141"/>
-        <v>188691.40557688577</v>
+        <f t="shared" ca="1" si="143"/>
+        <v>191340.79324579146</v>
       </c>
       <c r="I249" s="64">
-        <f t="shared" ca="1" si="141"/>
-        <v>220473.4339692666</v>
+        <f t="shared" ca="1" si="143"/>
+        <v>224123.56575857685</v>
       </c>
       <c r="J249" s="64">
-        <f t="shared" ca="1" si="141"/>
-        <v>253977.52520268637</v>
+        <f t="shared" ca="1" si="143"/>
+        <v>258677.46470421276</v>
       </c>
     </row>
     <row r="250" spans="1:10">
@@ -9723,28 +9753,28 @@
         <v>41733</v>
       </c>
       <c r="E251" s="64">
-        <f t="shared" ref="E251:J251" si="142">E27</f>
+        <f t="shared" ref="E251:J251" si="144">E27</f>
         <v>37037</v>
       </c>
       <c r="F251" s="64">
-        <f t="shared" ca="1" si="142"/>
-        <v>35963.454583861196</v>
+        <f t="shared" ca="1" si="144"/>
+        <v>37097.92463489787</v>
       </c>
       <c r="G251" s="64">
-        <f t="shared" ca="1" si="142"/>
-        <v>38128.155446655452</v>
+        <f t="shared" ca="1" si="144"/>
+        <v>39319.685709211175</v>
       </c>
       <c r="H251" s="64">
-        <f t="shared" ca="1" si="142"/>
-        <v>39846.827932532637</v>
+        <f t="shared" ca="1" si="144"/>
+        <v>41096.427450476993</v>
       </c>
       <c r="I251" s="64">
-        <f t="shared" ca="1" si="142"/>
-        <v>41818.458411027415</v>
+        <f t="shared" ca="1" si="144"/>
+        <v>43135.226990505573</v>
       </c>
       <c r="J251" s="64">
-        <f t="shared" ca="1" si="142"/>
-        <v>44084.330570289167</v>
+        <f t="shared" ca="1" si="144"/>
+        <v>45465.656507431544</v>
       </c>
     </row>
     <row r="252" spans="1:10">
@@ -9789,23 +9819,23 @@
       </c>
       <c r="F253" s="72">
         <f ca="1">-(F252*F251)</f>
-        <v>-10789.036375158359</v>
+        <v>-11129.377390469361</v>
       </c>
       <c r="G253" s="72">
         <f ca="1">-(G252*G251)</f>
-        <v>-9150.7573071973075</v>
+        <v>-9436.7245702106811</v>
       </c>
       <c r="H253" s="72">
         <f ca="1">-(H252*H251)</f>
-        <v>-9563.2387038078323</v>
+        <v>-9863.1425881144787</v>
       </c>
       <c r="I253" s="72">
         <f ca="1">-(I252*I251)</f>
-        <v>-10036.430018646579</v>
+        <v>-10352.454477721338</v>
       </c>
       <c r="J253" s="72">
         <f ca="1">-(J252*J251)</f>
-        <v>-10580.239336869399</v>
+        <v>-10911.75756178357</v>
       </c>
     </row>
     <row r="254" spans="1:10">
@@ -9844,19 +9874,19 @@
         <v>-471</v>
       </c>
       <c r="G256" s="96">
-        <f t="shared" ref="G256:J256" si="143">F258</f>
+        <f t="shared" ref="G256:J256" si="145">F258</f>
         <v>-471</v>
       </c>
       <c r="H256" s="96">
-        <f t="shared" si="143"/>
+        <f t="shared" si="145"/>
         <v>-471</v>
       </c>
       <c r="I256" s="96">
-        <f t="shared" si="143"/>
+        <f t="shared" si="145"/>
         <v>-471</v>
       </c>
       <c r="J256" s="96">
-        <f t="shared" si="143"/>
+        <f t="shared" si="145"/>
         <v>-471</v>
       </c>
     </row>
@@ -9901,19 +9931,19 @@
         <v>-471</v>
       </c>
       <c r="G258" s="96">
-        <f t="shared" ref="G258:J258" si="144">SUM(G256:G257)</f>
+        <f t="shared" ref="G258:J258" si="146">SUM(G256:G257)</f>
         <v>-471</v>
       </c>
       <c r="H258" s="96">
-        <f t="shared" si="144"/>
+        <f t="shared" si="146"/>
         <v>-471</v>
       </c>
       <c r="I258" s="96">
-        <f t="shared" si="144"/>
+        <f t="shared" si="146"/>
         <v>-471</v>
       </c>
       <c r="J258" s="96">
-        <f t="shared" si="144"/>
+        <f t="shared" si="146"/>
         <v>-471</v>
       </c>
     </row>
@@ -9940,31 +9970,31 @@
       </c>
       <c r="C261" s="80"/>
       <c r="D261" s="80">
-        <f t="shared" ref="D261:J262" si="145">D13</f>
+        <f t="shared" ref="D261:J262" si="147">D13</f>
         <v>2012</v>
       </c>
       <c r="E261" s="80">
-        <f t="shared" si="145"/>
+        <f t="shared" si="147"/>
         <v>2013</v>
       </c>
       <c r="F261" s="81">
-        <f t="shared" si="145"/>
+        <f t="shared" si="147"/>
         <v>2014</v>
       </c>
       <c r="G261" s="81">
-        <f t="shared" si="145"/>
+        <f t="shared" si="147"/>
         <v>2015</v>
       </c>
       <c r="H261" s="81">
-        <f t="shared" si="145"/>
+        <f t="shared" si="147"/>
         <v>2016</v>
       </c>
       <c r="I261" s="81">
-        <f t="shared" si="145"/>
+        <f t="shared" si="147"/>
         <v>2017</v>
       </c>
       <c r="J261" s="81">
-        <f t="shared" si="145"/>
+        <f t="shared" si="147"/>
         <v>2018</v>
       </c>
     </row>
@@ -9975,31 +10005,31 @@
       </c>
       <c r="C262" s="82"/>
       <c r="D262" s="82">
-        <f t="shared" si="145"/>
+        <f t="shared" si="147"/>
         <v>41181</v>
       </c>
       <c r="E262" s="82">
-        <f t="shared" si="145"/>
+        <f t="shared" si="147"/>
         <v>41545</v>
       </c>
       <c r="F262" s="82">
-        <f t="shared" si="145"/>
+        <f t="shared" si="147"/>
         <v>41912</v>
       </c>
       <c r="G262" s="82">
-        <f t="shared" si="145"/>
+        <f t="shared" si="147"/>
         <v>42277</v>
       </c>
       <c r="H262" s="82">
-        <f t="shared" si="145"/>
+        <f t="shared" si="147"/>
         <v>42643</v>
       </c>
       <c r="I262" s="82">
-        <f t="shared" si="145"/>
+        <f t="shared" si="147"/>
         <v>43008</v>
       </c>
       <c r="J262" s="82">
-        <f t="shared" si="145"/>
+        <f t="shared" si="147"/>
         <v>43373</v>
       </c>
     </row>
@@ -10021,23 +10051,23 @@
       <c r="E264"/>
       <c r="F264" s="52">
         <f ca="1">F27</f>
-        <v>35963.454583861196</v>
+        <v>37097.92463489787</v>
       </c>
       <c r="G264" s="52">
-        <f t="shared" ref="G264:J264" ca="1" si="146">G27</f>
-        <v>38128.155446655452</v>
+        <f t="shared" ref="G264:J264" ca="1" si="148">G27</f>
+        <v>39319.685709211175</v>
       </c>
       <c r="H264" s="52">
-        <f t="shared" ca="1" si="146"/>
-        <v>39846.827932532637</v>
+        <f t="shared" ca="1" si="148"/>
+        <v>41096.427450476993</v>
       </c>
       <c r="I264" s="52">
-        <f t="shared" ca="1" si="146"/>
-        <v>41818.458411027415</v>
+        <f t="shared" ca="1" si="148"/>
+        <v>43135.226990505573</v>
       </c>
       <c r="J264" s="52">
-        <f t="shared" ca="1" si="146"/>
-        <v>44084.330570289167</v>
+        <f t="shared" ca="1" si="148"/>
+        <v>45465.656507431544</v>
       </c>
     </row>
     <row r="265" spans="1:10">
@@ -10052,19 +10082,19 @@
         <v>7145.3176115999995</v>
       </c>
       <c r="G265" s="96">
-        <f t="shared" ref="G265:J265" si="147">G44</f>
+        <f t="shared" ref="G265:J265" si="149">G44</f>
         <v>7540.5401478143021</v>
       </c>
       <c r="H265" s="96">
-        <f t="shared" si="147"/>
+        <f t="shared" si="149"/>
         <v>7682.1924442956242</v>
       </c>
       <c r="I265" s="96">
-        <f t="shared" si="147"/>
+        <f t="shared" si="149"/>
         <v>7792.0651309652267</v>
       </c>
       <c r="J265" s="96">
-        <f t="shared" si="147"/>
+        <f t="shared" si="149"/>
         <v>8007.2119367516216</v>
       </c>
     </row>
@@ -10080,19 +10110,19 @@
         <v>2212.6002930107998</v>
       </c>
       <c r="G266" s="96">
-        <f t="shared" ref="G266:J266" si="148">G231</f>
+        <f t="shared" ref="G266:J266" si="150">G231</f>
         <v>2187.0654505218836</v>
       </c>
       <c r="H266" s="96">
-        <f t="shared" si="148"/>
+        <f t="shared" si="150"/>
         <v>2285.0340049994029</v>
       </c>
       <c r="I266" s="96">
-        <f t="shared" si="148"/>
+        <f t="shared" si="150"/>
         <v>2397.4217865745363</v>
       </c>
       <c r="J266" s="96">
-        <f t="shared" si="148"/>
+        <f t="shared" si="150"/>
         <v>2526.5820669059194</v>
       </c>
     </row>
@@ -10108,19 +10138,19 @@
         <v>-433.19057869999779</v>
       </c>
       <c r="G267" s="109">
-        <f t="shared" ref="G267:J267" si="149">-(G125)</f>
+        <f t="shared" ref="G267:J267" si="151">-(G125)</f>
         <v>-793.85892471924126</v>
       </c>
       <c r="H267" s="109">
-        <f t="shared" si="149"/>
+        <f t="shared" si="151"/>
         <v>-641.86294312857353</v>
       </c>
       <c r="I267" s="109">
-        <f t="shared" si="149"/>
+        <f t="shared" si="151"/>
         <v>-736.33374135432132</v>
       </c>
       <c r="J267" s="109">
-        <f t="shared" si="149"/>
+        <f t="shared" si="151"/>
         <v>-846.22252630906041</v>
       </c>
     </row>
@@ -10135,19 +10165,19 @@
         <v>-40.21401303359994</v>
       </c>
       <c r="G268" s="96">
-        <f t="shared" ref="G268:J268" si="150">-(G133)</f>
+        <f t="shared" ref="G268:J268" si="152">-(G133)</f>
         <v>-143.2169385561017</v>
       </c>
       <c r="H268" s="96">
-        <f t="shared" si="150"/>
+        <f t="shared" si="152"/>
         <v>-87.234241310197831</v>
       </c>
       <c r="I268" s="96">
-        <f t="shared" si="150"/>
+        <f t="shared" si="152"/>
         <v>-100.07356861116841</v>
       </c>
       <c r="J268" s="96">
-        <f t="shared" si="150"/>
+        <f t="shared" si="152"/>
         <v>-115.00832202955644</v>
       </c>
     </row>
@@ -10162,19 +10192,19 @@
         <v>523.96529036379798</v>
       </c>
       <c r="G269" s="96">
-        <f t="shared" ref="G269:J269" si="151">G141</f>
+        <f t="shared" ref="G269:J269" si="153">G141</f>
         <v>1422.4150749379296</v>
       </c>
       <c r="H269" s="96">
-        <f t="shared" si="151"/>
+        <f t="shared" si="153"/>
         <v>1089.1062854485281</v>
       </c>
       <c r="I269" s="96">
-        <f t="shared" si="151"/>
+        <f t="shared" si="153"/>
         <v>1249.4033414485275</v>
       </c>
       <c r="J269" s="96">
-        <f t="shared" si="151"/>
+        <f t="shared" si="153"/>
         <v>1435.8614750356755</v>
       </c>
     </row>
@@ -10189,19 +10219,19 @@
         <v>-72.551695800000743</v>
       </c>
       <c r="G270" s="96">
-        <f t="shared" ref="G270:J270" si="152">G149</f>
+        <f t="shared" ref="G270:J270" si="154">G149</f>
         <v>6.8775139912322629</v>
       </c>
       <c r="H270" s="96">
-        <f t="shared" si="152"/>
+        <f t="shared" si="154"/>
         <v>-15.057317766426422</v>
       </c>
       <c r="I270" s="96">
-        <f t="shared" si="152"/>
+        <f t="shared" si="154"/>
         <v>138.9493653205609</v>
       </c>
       <c r="J270" s="96">
-        <f t="shared" si="152"/>
+        <f t="shared" si="154"/>
         <v>-15.249989913376339</v>
       </c>
     </row>
@@ -10216,19 +10246,19 @@
         <v>0</v>
       </c>
       <c r="G271">
-        <f t="shared" ref="G271:J271" si="153">-(G257)</f>
+        <f t="shared" ref="G271:J271" si="155">-(G257)</f>
         <v>0</v>
       </c>
       <c r="H271">
-        <f t="shared" si="153"/>
+        <f t="shared" si="155"/>
         <v>0</v>
       </c>
       <c r="I271">
-        <f t="shared" si="153"/>
+        <f t="shared" si="155"/>
         <v>0</v>
       </c>
       <c r="J271">
-        <f t="shared" si="153"/>
+        <f t="shared" si="155"/>
         <v>0</v>
       </c>
     </row>
@@ -10243,19 +10273,19 @@
         <v>0</v>
       </c>
       <c r="G272">
-        <f t="shared" ref="G272:J272" si="154">-(G191)</f>
+        <f t="shared" ref="G272:J272" si="156">-(G191)</f>
         <v>0</v>
       </c>
       <c r="H272">
-        <f t="shared" si="154"/>
+        <f t="shared" si="156"/>
         <v>0</v>
       </c>
       <c r="I272">
-        <f t="shared" si="154"/>
+        <f t="shared" si="156"/>
         <v>0</v>
       </c>
       <c r="J272">
-        <f t="shared" si="154"/>
+        <f t="shared" si="156"/>
         <v>0</v>
       </c>
     </row>
@@ -10270,19 +10300,19 @@
         <v>0</v>
       </c>
       <c r="G273">
-        <f t="shared" ref="G273:J273" si="155">-(G196)</f>
+        <f t="shared" ref="G273:J273" si="157">-(G196)</f>
         <v>0</v>
       </c>
       <c r="H273">
-        <f t="shared" si="155"/>
+        <f t="shared" si="157"/>
         <v>0</v>
       </c>
       <c r="I273">
-        <f t="shared" si="155"/>
+        <f t="shared" si="157"/>
         <v>0</v>
       </c>
       <c r="J273">
-        <f t="shared" si="155"/>
+        <f t="shared" si="157"/>
         <v>0</v>
       </c>
     </row>
@@ -10297,19 +10327,19 @@
         <v>3000</v>
       </c>
       <c r="G274" s="96">
-        <f t="shared" ref="G274:J274" si="156">G201</f>
+        <f t="shared" ref="G274:J274" si="158">G201</f>
         <v>3000</v>
       </c>
       <c r="H274" s="96">
-        <f t="shared" si="156"/>
+        <f t="shared" si="158"/>
         <v>3000</v>
       </c>
       <c r="I274" s="96">
-        <f t="shared" si="156"/>
+        <f t="shared" si="158"/>
         <v>3000</v>
       </c>
       <c r="J274" s="96">
-        <f t="shared" si="156"/>
+        <f t="shared" si="158"/>
         <v>3000</v>
       </c>
     </row>
@@ -10324,19 +10354,19 @@
         <v>0</v>
       </c>
       <c r="G275">
-        <f t="shared" ref="G275:J275" si="157">G211</f>
+        <f t="shared" ref="G275:J275" si="159">G211</f>
         <v>0</v>
       </c>
       <c r="H275">
-        <f t="shared" si="157"/>
+        <f t="shared" si="159"/>
         <v>0</v>
       </c>
       <c r="I275">
-        <f t="shared" si="157"/>
+        <f t="shared" si="159"/>
         <v>0</v>
       </c>
       <c r="J275">
-        <f t="shared" si="157"/>
+        <f t="shared" si="159"/>
         <v>0</v>
       </c>
     </row>
@@ -10348,23 +10378,23 @@
       <c r="E276"/>
       <c r="F276" s="127">
         <f ca="1">SUM(F264:F275)</f>
-        <v>48299.381491302192</v>
+        <v>49433.851542338874</v>
       </c>
       <c r="G276" s="127">
-        <f t="shared" ref="G276:J276" ca="1" si="158">SUM(G264:G275)</f>
-        <v>51347.977770645462</v>
+        <f t="shared" ref="G276:J276" ca="1" si="160">SUM(G264:G275)</f>
+        <v>52539.508033201186</v>
       </c>
       <c r="H276" s="127">
-        <f t="shared" ca="1" si="158"/>
-        <v>53159.006165070998</v>
+        <f t="shared" ca="1" si="160"/>
+        <v>54408.605683015354</v>
       </c>
       <c r="I276" s="127">
-        <f t="shared" ca="1" si="158"/>
-        <v>55559.890725370773</v>
+        <f t="shared" ca="1" si="160"/>
+        <v>56876.65930484893</v>
       </c>
       <c r="J276" s="127">
-        <f t="shared" ca="1" si="158"/>
-        <v>58077.505210730385</v>
+        <f t="shared" ca="1" si="160"/>
+        <v>59458.831147872763</v>
       </c>
     </row>
     <row r="277" spans="2:12">
@@ -10388,19 +10418,19 @@
         <v>-8963.7023699999991</v>
       </c>
       <c r="G278" s="96">
-        <f t="shared" ref="G278:J278" si="159">-(G171)</f>
+        <f t="shared" ref="G278:J278" si="161">-(G171)</f>
         <v>-10746.78712756443</v>
       </c>
       <c r="H278" s="96">
-        <f t="shared" si="159"/>
+        <f t="shared" si="161"/>
         <v>-11228.18433491086</v>
       </c>
       <c r="I278" s="96">
-        <f t="shared" si="159"/>
+        <f t="shared" si="161"/>
         <v>-11780.434640926602</v>
       </c>
       <c r="J278" s="96">
-        <f t="shared" si="159"/>
+        <f t="shared" si="161"/>
         <v>-12415.101535658396</v>
       </c>
     </row>
@@ -10415,19 +10445,19 @@
         <v>0</v>
       </c>
       <c r="G279">
-        <f t="shared" ref="G279:J279" si="160">-(G159)</f>
+        <f t="shared" ref="G279:J279" si="162">-(G159)</f>
         <v>0</v>
       </c>
       <c r="H279">
-        <f t="shared" si="160"/>
+        <f t="shared" si="162"/>
         <v>0</v>
       </c>
       <c r="I279">
-        <f t="shared" si="160"/>
+        <f t="shared" si="162"/>
         <v>0</v>
       </c>
       <c r="J279">
-        <f t="shared" si="160"/>
+        <f t="shared" si="162"/>
         <v>0</v>
       </c>
     </row>
@@ -10442,19 +10472,19 @@
         <v>-8963.7023699999991</v>
       </c>
       <c r="G280" s="128">
-        <f t="shared" ref="G280:J280" si="161">SUM(G278:G279)</f>
+        <f t="shared" ref="G280:J280" si="163">SUM(G278:G279)</f>
         <v>-10746.78712756443</v>
       </c>
       <c r="H280" s="128">
-        <f t="shared" si="161"/>
+        <f t="shared" si="163"/>
         <v>-11228.18433491086</v>
       </c>
       <c r="I280" s="128">
-        <f t="shared" si="161"/>
+        <f t="shared" si="163"/>
         <v>-11780.434640926602</v>
       </c>
       <c r="J280" s="128">
-        <f t="shared" si="161"/>
+        <f t="shared" si="163"/>
         <v>-12415.101535658396</v>
       </c>
     </row>
@@ -10479,19 +10509,19 @@
         <v>0</v>
       </c>
       <c r="G282" s="70">
-        <f t="shared" ref="G282:J282" si="162">G210</f>
+        <f t="shared" ref="G282:J282" si="164">G210</f>
         <v>0</v>
       </c>
       <c r="H282" s="70">
-        <f t="shared" si="162"/>
+        <f t="shared" si="164"/>
         <v>-2500</v>
       </c>
       <c r="I282" s="70">
-        <f t="shared" si="162"/>
+        <f t="shared" si="164"/>
         <v>0</v>
       </c>
       <c r="J282" s="70">
-        <f t="shared" si="162"/>
+        <f t="shared" si="164"/>
         <v>-6000</v>
       </c>
     </row>
@@ -10503,23 +10533,23 @@
       <c r="E283"/>
       <c r="F283" s="96">
         <f ca="1">F248</f>
-        <v>-10789.036375158359</v>
+        <v>-11129.377390469361</v>
       </c>
       <c r="G283" s="96">
-        <f t="shared" ref="G283:J283" ca="1" si="163">G248</f>
-        <v>-9150.7573071973075</v>
+        <f t="shared" ref="G283:J283" ca="1" si="165">G248</f>
+        <v>-9436.7245702106811</v>
       </c>
       <c r="H283" s="96">
-        <f t="shared" ca="1" si="163"/>
-        <v>-9563.2387038078323</v>
+        <f t="shared" ca="1" si="165"/>
+        <v>-9863.1425881144569</v>
       </c>
       <c r="I283" s="96">
-        <f t="shared" ca="1" si="163"/>
-        <v>-10036.430018646579</v>
+        <f t="shared" ca="1" si="165"/>
+        <v>-10352.454477721536</v>
       </c>
       <c r="J283" s="96">
-        <f t="shared" ca="1" si="163"/>
-        <v>-10580.239336869399</v>
+        <f t="shared" ca="1" si="165"/>
+        <v>-10911.757561782981</v>
       </c>
       <c r="L283" s="116"/>
     </row>
@@ -10534,19 +10564,19 @@
         <v>0</v>
       </c>
       <c r="G284">
-        <f t="shared" ref="G284:J284" si="164">G226</f>
+        <f t="shared" ref="G284:J284" si="166">G226</f>
         <v>0</v>
       </c>
       <c r="H284">
-        <f t="shared" si="164"/>
+        <f t="shared" si="166"/>
         <v>0</v>
       </c>
       <c r="I284">
-        <f t="shared" si="164"/>
+        <f t="shared" si="166"/>
         <v>0</v>
       </c>
       <c r="J284">
-        <f t="shared" si="164"/>
+        <f t="shared" si="166"/>
         <v>0</v>
       </c>
     </row>
@@ -10561,19 +10591,19 @@
         <v>-23968</v>
       </c>
       <c r="G285" s="96">
-        <f t="shared" ref="G285:J285" si="165">G239</f>
+        <f t="shared" ref="G285:J285" si="167">G239</f>
         <v>-23968</v>
       </c>
       <c r="H285" s="96">
-        <f t="shared" si="165"/>
+        <f t="shared" si="167"/>
         <v>-23968</v>
       </c>
       <c r="I285" s="96">
-        <f t="shared" si="165"/>
+        <f t="shared" si="167"/>
         <v>-23968</v>
       </c>
       <c r="J285" s="96">
-        <f t="shared" si="165"/>
+        <f t="shared" si="167"/>
         <v>-23968</v>
       </c>
     </row>
@@ -10588,19 +10618,19 @@
         <v>0</v>
       </c>
       <c r="G286">
-        <f t="shared" ref="G286:J286" si="166">G257</f>
+        <f t="shared" ref="G286:J286" si="168">G257</f>
         <v>0</v>
       </c>
       <c r="H286">
-        <f t="shared" si="166"/>
+        <f t="shared" si="168"/>
         <v>0</v>
       </c>
       <c r="I286">
-        <f t="shared" si="166"/>
+        <f t="shared" si="168"/>
         <v>0</v>
       </c>
       <c r="J286">
-        <f t="shared" si="166"/>
+        <f t="shared" si="168"/>
         <v>0</v>
       </c>
     </row>
@@ -10639,23 +10669,23 @@
       <c r="E288"/>
       <c r="F288" s="128">
         <f ca="1">SUM(F282:F287)</f>
-        <v>-34757.036375158357</v>
+        <v>-35097.377390469359</v>
       </c>
       <c r="G288" s="128">
-        <f t="shared" ref="G288:J288" ca="1" si="167">SUM(G282:G287)</f>
-        <v>-33118.757307197309</v>
+        <f t="shared" ref="G288:J288" ca="1" si="169">SUM(G282:G287)</f>
+        <v>-33404.724570210681</v>
       </c>
       <c r="H288" s="128">
-        <f t="shared" ca="1" si="167"/>
-        <v>-36031.23870380783</v>
+        <f t="shared" ca="1" si="169"/>
+        <v>-36331.142588114453</v>
       </c>
       <c r="I288" s="128">
-        <f t="shared" ca="1" si="167"/>
-        <v>-34004.430018646577</v>
+        <f t="shared" ca="1" si="169"/>
+        <v>-34320.454477721534</v>
       </c>
       <c r="J288" s="128">
-        <f t="shared" ca="1" si="167"/>
-        <v>-40548.239336869403</v>
+        <f t="shared" ca="1" si="169"/>
+        <v>-40879.757561782979</v>
       </c>
     </row>
     <row r="289" spans="1:10">
@@ -10675,23 +10705,23 @@
       <c r="E290"/>
       <c r="F290" s="128">
         <f ca="1">SUM(F288,F280,F276)</f>
-        <v>4578.6427461438361</v>
+        <v>5372.7717818695164</v>
       </c>
       <c r="G290" s="128">
-        <f t="shared" ref="G290:J290" ca="1" si="168">SUM(G288,G280,G276)</f>
-        <v>7482.4333358837248</v>
+        <f t="shared" ref="G290:J290" ca="1" si="170">SUM(G288,G280,G276)</f>
+        <v>8387.9963354260763</v>
       </c>
       <c r="H290" s="128">
-        <f t="shared" ca="1" si="168"/>
-        <v>5899.5831263523069</v>
+        <f t="shared" ca="1" si="170"/>
+        <v>6849.2787599900403</v>
       </c>
       <c r="I290" s="128">
-        <f t="shared" ca="1" si="168"/>
-        <v>9775.0260657975959</v>
+        <f t="shared" ca="1" si="170"/>
+        <v>10775.770186200796</v>
       </c>
       <c r="J290" s="128">
-        <f t="shared" ca="1" si="168"/>
-        <v>5114.1643382025868</v>
+        <f t="shared" ca="1" si="170"/>
+        <v>6163.9720504313882</v>
       </c>
     </row>
     <row r="292" spans="1:10">
@@ -10717,31 +10747,31 @@
       </c>
       <c r="C293" s="80"/>
       <c r="D293" s="80">
-        <f t="shared" ref="D293:J294" si="169">D13</f>
+        <f t="shared" ref="D293:J294" si="171">D13</f>
         <v>2012</v>
       </c>
       <c r="E293" s="80">
-        <f t="shared" si="169"/>
+        <f t="shared" si="171"/>
         <v>2013</v>
       </c>
       <c r="F293" s="81">
-        <f t="shared" si="169"/>
+        <f t="shared" si="171"/>
         <v>2014</v>
       </c>
       <c r="G293" s="81">
-        <f t="shared" si="169"/>
+        <f t="shared" si="171"/>
         <v>2015</v>
       </c>
       <c r="H293" s="81">
-        <f t="shared" si="169"/>
+        <f t="shared" si="171"/>
         <v>2016</v>
       </c>
       <c r="I293" s="81">
-        <f t="shared" si="169"/>
+        <f t="shared" si="171"/>
         <v>2017</v>
       </c>
       <c r="J293" s="81">
-        <f t="shared" si="169"/>
+        <f t="shared" si="171"/>
         <v>2018</v>
       </c>
     </row>
@@ -10752,31 +10782,31 @@
       </c>
       <c r="C294" s="82"/>
       <c r="D294" s="82">
-        <f t="shared" si="169"/>
+        <f t="shared" si="171"/>
         <v>41181</v>
       </c>
       <c r="E294" s="82">
-        <f t="shared" si="169"/>
+        <f t="shared" si="171"/>
         <v>41545</v>
       </c>
       <c r="F294" s="82">
-        <f t="shared" si="169"/>
+        <f t="shared" si="171"/>
         <v>41912</v>
       </c>
       <c r="G294" s="82">
-        <f t="shared" si="169"/>
+        <f t="shared" si="171"/>
         <v>42277</v>
       </c>
       <c r="H294" s="82">
-        <f t="shared" si="169"/>
+        <f t="shared" si="171"/>
         <v>42643</v>
       </c>
       <c r="I294" s="82">
-        <f t="shared" si="169"/>
+        <f t="shared" si="171"/>
         <v>43008</v>
       </c>
       <c r="J294" s="82">
-        <f t="shared" si="169"/>
+        <f t="shared" si="171"/>
         <v>43373</v>
       </c>
     </row>
@@ -10801,24 +10831,24 @@
       </c>
       <c r="D297"/>
       <c r="E297"/>
-      <c r="F297" s="96">
+      <c r="F297" s="72">
         <f>E299</f>
         <v>0</v>
       </c>
-      <c r="G297" s="96">
-        <f t="shared" ref="G297:J297" ca="1" si="170">F299</f>
-        <v>0</v>
-      </c>
-      <c r="H297" s="96">
-        <f t="shared" ca="1" si="170"/>
-        <v>0</v>
-      </c>
-      <c r="I297" s="96">
-        <f t="shared" ca="1" si="170"/>
-        <v>0</v>
-      </c>
-      <c r="J297" s="96">
-        <f t="shared" ca="1" si="170"/>
+      <c r="G297" s="72">
+        <f t="shared" ref="G297:J297" ca="1" si="172">F299</f>
+        <v>0</v>
+      </c>
+      <c r="H297" s="72">
+        <f t="shared" ca="1" si="172"/>
+        <v>0</v>
+      </c>
+      <c r="I297" s="72">
+        <f t="shared" ca="1" si="172"/>
+        <v>0</v>
+      </c>
+      <c r="J297" s="72">
+        <f t="shared" ca="1" si="172"/>
         <v>0</v>
       </c>
     </row>
@@ -10828,24 +10858,24 @@
       </c>
       <c r="D298"/>
       <c r="E298"/>
-      <c r="F298" s="96">
+      <c r="F298" s="72">
         <f ca="1">-MIN(F297,F309)</f>
         <v>0</v>
       </c>
-      <c r="G298" s="96">
-        <f t="shared" ref="G298:J298" ca="1" si="171">-MIN(G297,G309)</f>
-        <v>0</v>
-      </c>
-      <c r="H298" s="96">
-        <f t="shared" ca="1" si="171"/>
-        <v>0</v>
-      </c>
-      <c r="I298" s="96">
-        <f t="shared" ca="1" si="171"/>
-        <v>0</v>
-      </c>
-      <c r="J298" s="96">
-        <f t="shared" ca="1" si="171"/>
+      <c r="G298" s="72">
+        <f t="shared" ref="G298:J298" ca="1" si="173">-MIN(G297,G309)</f>
+        <v>0</v>
+      </c>
+      <c r="H298" s="72">
+        <f t="shared" ca="1" si="173"/>
+        <v>0</v>
+      </c>
+      <c r="I298" s="72">
+        <f t="shared" ca="1" si="173"/>
+        <v>0</v>
+      </c>
+      <c r="J298" s="72">
+        <f t="shared" ca="1" si="173"/>
         <v>0</v>
       </c>
     </row>
@@ -10853,32 +10883,32 @@
       <c r="B299" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="D299" s="96">
+      <c r="D299" s="72">
         <f>D99</f>
         <v>0</v>
       </c>
-      <c r="E299" s="96">
+      <c r="E299" s="72">
         <f>E99</f>
         <v>0</v>
       </c>
-      <c r="F299" s="96">
+      <c r="F299" s="72">
         <f ca="1">SUM(F297:F298)</f>
         <v>0</v>
       </c>
-      <c r="G299" s="96">
-        <f t="shared" ref="G299:J299" ca="1" si="172">SUM(G297:G298)</f>
-        <v>0</v>
-      </c>
-      <c r="H299" s="96">
-        <f t="shared" ca="1" si="172"/>
-        <v>0</v>
-      </c>
-      <c r="I299" s="96">
-        <f t="shared" ca="1" si="172"/>
-        <v>0</v>
-      </c>
-      <c r="J299" s="96">
-        <f t="shared" ca="1" si="172"/>
+      <c r="G299" s="72">
+        <f t="shared" ref="G299:J299" ca="1" si="174">SUM(G297:G298)</f>
+        <v>0</v>
+      </c>
+      <c r="H299" s="72">
+        <f t="shared" ca="1" si="174"/>
+        <v>0</v>
+      </c>
+      <c r="I299" s="72">
+        <f t="shared" ca="1" si="174"/>
+        <v>0</v>
+      </c>
+      <c r="J299" s="72">
+        <f t="shared" ca="1" si="174"/>
         <v>0</v>
       </c>
     </row>
@@ -10898,24 +10928,24 @@
       </c>
       <c r="D301"/>
       <c r="E301"/>
-      <c r="F301" s="109">
+      <c r="F301" s="108">
         <f>SUM(F88:F89)</f>
         <v>15339.404591733597</v>
       </c>
-      <c r="G301" s="109">
-        <f t="shared" ref="G301:J301" si="173">SUM(G88:G89)</f>
+      <c r="G301" s="108">
+        <f t="shared" ref="G301:J301" si="175">SUM(G88:G89)</f>
         <v>16276.480455008941</v>
       </c>
-      <c r="H301" s="109">
-        <f t="shared" si="173"/>
+      <c r="H301" s="108">
+        <f t="shared" si="175"/>
         <v>17005.577639447711</v>
       </c>
-      <c r="I301" s="109">
-        <f t="shared" si="173"/>
+      <c r="I301" s="108">
+        <f t="shared" si="175"/>
         <v>17841.984949413203</v>
       </c>
-      <c r="J301" s="109">
-        <f t="shared" si="173"/>
+      <c r="J301" s="108">
+        <f t="shared" si="175"/>
         <v>18803.215797751818</v>
       </c>
     </row>
@@ -10930,19 +10960,19 @@
         <v>OK</v>
       </c>
       <c r="G302" s="131" t="str">
-        <f t="shared" ref="G302:J302" ca="1" si="174">IF(G299&gt;G301,"OVERDRAWN","OK")</f>
+        <f t="shared" ref="G302:J302" ca="1" si="176">IF(G299&gt;G301,"OVERDRAWN","OK")</f>
         <v>OK</v>
       </c>
       <c r="H302" s="131" t="str">
-        <f t="shared" ca="1" si="174"/>
+        <f t="shared" ca="1" si="176"/>
         <v>OK</v>
       </c>
       <c r="I302" s="131" t="str">
-        <f t="shared" ca="1" si="174"/>
+        <f t="shared" ca="1" si="176"/>
         <v>OK</v>
       </c>
       <c r="J302" s="131" t="str">
-        <f t="shared" ca="1" si="174"/>
+        <f t="shared" ca="1" si="176"/>
         <v>OK</v>
       </c>
     </row>
@@ -10974,25 +11004,25 @@
       </c>
       <c r="D305"/>
       <c r="E305"/>
-      <c r="F305" s="96">
+      <c r="F305" s="72">
         <f>E87</f>
         <v>146761</v>
       </c>
-      <c r="G305" s="96">
-        <f t="shared" ref="G305:J305" si="175">F87</f>
-        <v>0</v>
-      </c>
-      <c r="H305" s="96">
-        <f t="shared" si="175"/>
-        <v>0</v>
-      </c>
-      <c r="I305" s="96">
-        <f t="shared" si="175"/>
-        <v>0</v>
-      </c>
-      <c r="J305" s="96">
-        <f t="shared" si="175"/>
-        <v>0</v>
+      <c r="G305" s="72">
+        <f t="shared" ref="G305:J305" ca="1" si="177">F87</f>
+        <v>152133.77178186952</v>
+      </c>
+      <c r="H305" s="72">
+        <f t="shared" ca="1" si="177"/>
+        <v>160521.76811729561</v>
+      </c>
+      <c r="I305" s="72">
+        <f t="shared" ca="1" si="177"/>
+        <v>167371.04687728541</v>
+      </c>
+      <c r="J305" s="72">
+        <f t="shared" ca="1" si="177"/>
+        <v>178146.81706348865</v>
       </c>
     </row>
     <row r="306" spans="2:10">
@@ -11001,19 +11031,19 @@
       </c>
       <c r="D306"/>
       <c r="E306"/>
-      <c r="F306" s="70">
+      <c r="F306" s="76">
         <v>5000</v>
       </c>
-      <c r="G306" s="70">
+      <c r="G306" s="76">
         <v>5000</v>
       </c>
-      <c r="H306" s="70">
+      <c r="H306" s="76">
         <v>5000</v>
       </c>
-      <c r="I306" s="70">
+      <c r="I306" s="76">
         <v>5000</v>
       </c>
-      <c r="J306" s="70">
+      <c r="J306" s="76">
         <v>5000</v>
       </c>
     </row>
@@ -11023,25 +11053,25 @@
       </c>
       <c r="D307"/>
       <c r="E307"/>
-      <c r="F307" s="96">
+      <c r="F307" s="72">
         <f>F305-F306</f>
         <v>141761</v>
       </c>
-      <c r="G307" s="96">
-        <f t="shared" ref="G307:J307" si="176">G305-G306</f>
-        <v>-5000</v>
-      </c>
-      <c r="H307" s="96">
-        <f t="shared" si="176"/>
-        <v>-5000</v>
-      </c>
-      <c r="I307" s="96">
-        <f t="shared" si="176"/>
-        <v>-5000</v>
-      </c>
-      <c r="J307" s="96">
-        <f t="shared" si="176"/>
-        <v>-5000</v>
+      <c r="G307" s="72">
+        <f t="shared" ref="G307:J307" ca="1" si="178">G305-G306</f>
+        <v>147133.77178186952</v>
+      </c>
+      <c r="H307" s="72">
+        <f t="shared" ca="1" si="178"/>
+        <v>155521.76811729561</v>
+      </c>
+      <c r="I307" s="72">
+        <f t="shared" ca="1" si="178"/>
+        <v>162371.04687728541</v>
+      </c>
+      <c r="J307" s="72">
+        <f t="shared" ca="1" si="178"/>
+        <v>173146.81706348865</v>
       </c>
     </row>
     <row r="308" spans="2:10">
@@ -11050,25 +11080,25 @@
       </c>
       <c r="D308"/>
       <c r="E308"/>
-      <c r="F308" s="96">
+      <c r="F308" s="72">
         <f ca="1">SUM(F282:F286,F280,F276)</f>
-        <v>4578.6427461438361</v>
-      </c>
-      <c r="G308" s="96">
-        <f t="shared" ref="G308:J308" ca="1" si="177">SUM(G282:G286,G280,G276)</f>
-        <v>7482.4333358837248</v>
-      </c>
-      <c r="H308" s="96">
-        <f t="shared" ca="1" si="177"/>
-        <v>5899.5831263523069</v>
-      </c>
-      <c r="I308" s="96">
-        <f t="shared" ca="1" si="177"/>
-        <v>9775.0260657975959</v>
-      </c>
-      <c r="J308" s="96">
-        <f t="shared" ca="1" si="177"/>
-        <v>5114.1643382025868</v>
+        <v>5372.7717818695164</v>
+      </c>
+      <c r="G308" s="72">
+        <f t="shared" ref="G308:J308" ca="1" si="179">SUM(G282:G286,G280,G276)</f>
+        <v>8387.9963354260763</v>
+      </c>
+      <c r="H308" s="72">
+        <f t="shared" ca="1" si="179"/>
+        <v>6849.2787599900403</v>
+      </c>
+      <c r="I308" s="72">
+        <f t="shared" ca="1" si="179"/>
+        <v>10775.770186200796</v>
+      </c>
+      <c r="J308" s="72">
+        <f t="shared" ca="1" si="179"/>
+        <v>6163.9720504313882</v>
       </c>
     </row>
     <row r="309" spans="2:10">
@@ -11077,25 +11107,25 @@
       </c>
       <c r="D309"/>
       <c r="E309"/>
-      <c r="F309" s="96">
+      <c r="F309" s="72">
         <f ca="1">SUM(F307:F308)</f>
-        <v>146339.64274614383</v>
-      </c>
-      <c r="G309" s="96">
-        <f t="shared" ref="G309:J309" ca="1" si="178">SUM(G307:G308)</f>
-        <v>2482.4333358837248</v>
-      </c>
-      <c r="H309" s="96">
-        <f t="shared" ca="1" si="178"/>
-        <v>899.58312635230686</v>
-      </c>
-      <c r="I309" s="96">
-        <f t="shared" ca="1" si="178"/>
-        <v>4775.0260657975959</v>
-      </c>
-      <c r="J309" s="96">
-        <f t="shared" ca="1" si="178"/>
-        <v>114.1643382025868</v>
+        <v>147133.77178186952</v>
+      </c>
+      <c r="G309" s="72">
+        <f t="shared" ref="G309:J309" ca="1" si="180">SUM(G307:G308)</f>
+        <v>155521.76811729561</v>
+      </c>
+      <c r="H309" s="72">
+        <f t="shared" ca="1" si="180"/>
+        <v>162371.04687728564</v>
+      </c>
+      <c r="I309" s="72">
+        <f t="shared" ca="1" si="180"/>
+        <v>173146.8170634862</v>
+      </c>
+      <c r="J309" s="72">
+        <f t="shared" ca="1" si="180"/>
+        <v>179310.78911392004</v>
       </c>
     </row>
     <row r="310" spans="2:10">
@@ -11114,19 +11144,19 @@
       </c>
       <c r="D311"/>
       <c r="E311"/>
-      <c r="F311" s="56">
+      <c r="F311" s="69">
         <v>0.02</v>
       </c>
-      <c r="G311" s="56">
+      <c r="G311" s="69">
         <v>0.02</v>
       </c>
-      <c r="H311" s="56">
+      <c r="H311" s="69">
         <v>0.02</v>
       </c>
-      <c r="I311" s="56">
+      <c r="I311" s="69">
         <v>0.02</v>
       </c>
-      <c r="J311" s="56">
+      <c r="J311" s="69">
         <v>0.02</v>
       </c>
     </row>
@@ -11136,24 +11166,24 @@
       </c>
       <c r="D312"/>
       <c r="E312"/>
-      <c r="F312">
+      <c r="F312" s="68">
         <f ca="1">F311*AVERAGE(F297,F299)</f>
         <v>0</v>
       </c>
-      <c r="G312">
-        <f t="shared" ref="G312:J312" ca="1" si="179">G311*AVERAGE(G297,G299)</f>
-        <v>0</v>
-      </c>
-      <c r="H312">
-        <f t="shared" ca="1" si="179"/>
-        <v>0</v>
-      </c>
-      <c r="I312">
-        <f t="shared" ca="1" si="179"/>
-        <v>0</v>
-      </c>
-      <c r="J312">
-        <f t="shared" ca="1" si="179"/>
+      <c r="G312" s="68">
+        <f t="shared" ref="G312:J312" ca="1" si="181">G311*AVERAGE(G297,G299)</f>
+        <v>0</v>
+      </c>
+      <c r="H312" s="68">
+        <f t="shared" ca="1" si="181"/>
+        <v>0</v>
+      </c>
+      <c r="I312" s="68">
+        <f t="shared" ca="1" si="181"/>
+        <v>0</v>
+      </c>
+      <c r="J312" s="68">
+        <f t="shared" ca="1" si="181"/>
         <v>0</v>
       </c>
     </row>
@@ -11169,11 +11199,26 @@
       <c r="C315"/>
       <c r="D315"/>
       <c r="E315"/>
-      <c r="F315"/>
-      <c r="G315"/>
-      <c r="H315"/>
-      <c r="I315"/>
-      <c r="J315"/>
+      <c r="F315" s="72">
+        <f>E317</f>
+        <v>146761</v>
+      </c>
+      <c r="G315" s="72">
+        <f t="shared" ref="G315:J315" ca="1" si="182">F317</f>
+        <v>152133.77178186952</v>
+      </c>
+      <c r="H315" s="72">
+        <f t="shared" ca="1" si="182"/>
+        <v>160521.76811729555</v>
+      </c>
+      <c r="I315" s="72">
+        <f t="shared" ca="1" si="182"/>
+        <v>167371.04687728718</v>
+      </c>
+      <c r="J315" s="72">
+        <f t="shared" ca="1" si="182"/>
+        <v>178146.8170634683</v>
+      </c>
     </row>
     <row r="316" spans="2:10">
       <c r="B316" s="132" t="s">
@@ -11182,24 +11227,60 @@
       <c r="C316"/>
       <c r="D316"/>
       <c r="E316"/>
-      <c r="F316"/>
-      <c r="G316"/>
-      <c r="H316"/>
-      <c r="I316"/>
-      <c r="J316"/>
+      <c r="F316" s="72">
+        <f ca="1">F317-F315</f>
+        <v>5372.7717818695237</v>
+      </c>
+      <c r="G316" s="72">
+        <f t="shared" ref="G316:J316" ca="1" si="183">G317-G315</f>
+        <v>8387.9963354260253</v>
+      </c>
+      <c r="H316" s="72">
+        <f t="shared" ca="1" si="183"/>
+        <v>6849.2787599916337</v>
+      </c>
+      <c r="I316" s="72">
+        <f t="shared" ca="1" si="183"/>
+        <v>10775.770186181122</v>
+      </c>
+      <c r="J316" s="72">
+        <f t="shared" ca="1" si="183"/>
+        <v>6163.9720504382276</v>
+      </c>
     </row>
     <row r="317" spans="2:10">
       <c r="B317" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="C317"/>
-      <c r="D317"/>
-      <c r="E317"/>
-      <c r="F317"/>
-      <c r="G317"/>
-      <c r="H317"/>
-      <c r="I317"/>
-      <c r="J317"/>
+      <c r="C317" s="96"/>
+      <c r="D317" s="72">
+        <f>D87</f>
+        <v>121251</v>
+      </c>
+      <c r="E317" s="72">
+        <f>E87</f>
+        <v>146761</v>
+      </c>
+      <c r="F317" s="72">
+        <f ca="1">F87</f>
+        <v>152133.77178186952</v>
+      </c>
+      <c r="G317" s="72">
+        <f t="shared" ref="G317:J317" ca="1" si="184">G87</f>
+        <v>160521.76811729561</v>
+      </c>
+      <c r="H317" s="72">
+        <f t="shared" ca="1" si="184"/>
+        <v>167371.04687728541</v>
+      </c>
+      <c r="I317" s="72">
+        <f t="shared" ca="1" si="184"/>
+        <v>178146.81706348865</v>
+      </c>
+      <c r="J317" s="72">
+        <f t="shared" ca="1" si="184"/>
+        <v>184310.78911391232</v>
+      </c>
     </row>
     <row r="318" spans="2:10">
       <c r="B318" s="20"/>
@@ -11217,26 +11298,59 @@
         <v>159</v>
       </c>
       <c r="C319"/>
-      <c r="D319"/>
-      <c r="E319"/>
-      <c r="F319"/>
-      <c r="G319"/>
-      <c r="H319"/>
-      <c r="I319"/>
-      <c r="J319"/>
+      <c r="D319" s="56"/>
+      <c r="E319" s="133">
+        <v>1.03E-2</v>
+      </c>
+      <c r="F319" s="133">
+        <v>1.03E-2</v>
+      </c>
+      <c r="G319" s="133">
+        <v>1.03E-2</v>
+      </c>
+      <c r="H319" s="133">
+        <v>1.03E-2</v>
+      </c>
+      <c r="I319" s="133">
+        <v>1.03E-2</v>
+      </c>
+      <c r="J319" s="133">
+        <v>1.03E-2</v>
+      </c>
     </row>
     <row r="320" spans="2:10">
       <c r="B320" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C320"/>
-      <c r="D320"/>
-      <c r="E320"/>
-      <c r="F320"/>
-      <c r="G320"/>
-      <c r="H320"/>
-      <c r="I320"/>
-      <c r="J320"/>
+      <c r="C320" s="64"/>
+      <c r="D320" s="64">
+        <f t="shared" ref="D320:E320" si="185">D22</f>
+        <v>1088</v>
+      </c>
+      <c r="E320" s="64">
+        <f t="shared" si="185"/>
+        <v>1616</v>
+      </c>
+      <c r="F320" s="72">
+        <f ca="1">AVERAGE(F317,F315)*F319</f>
+        <v>1539.3080746766282</v>
+      </c>
+      <c r="G320" s="72">
+        <f t="shared" ref="G320:J320" ca="1" si="186">AVERAGE(G317,G315)*G319</f>
+        <v>1610.1760304807005</v>
+      </c>
+      <c r="H320" s="72">
+        <f t="shared" ca="1" si="186"/>
+        <v>1688.6479972220918</v>
+      </c>
+      <c r="I320" s="72">
+        <f t="shared" ca="1" si="186"/>
+        <v>1779.4169992949958</v>
+      </c>
+      <c r="J320" s="72">
+        <f t="shared" ca="1" si="186"/>
+        <v>1866.6566718135105</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B40">

</xml_diff>